<commit_message>
Changed methods in Change password,Request Token and Forgot Email
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNI-Automation web\clone_03_12_2021\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (13-12-2-2021)(2)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB54B22-E58A-4006-A7EB-3B8CF44DA4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C32803-362F-412F-AA0C-F206A857A741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId3"/>
     <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId4"/>
     <sheet name="forgotEmail" sheetId="6" r:id="rId5"/>
-    <sheet name="filters" sheetId="3" r:id="rId6"/>
-    <sheet name="profile" sheetId="2" r:id="rId7"/>
+    <sheet name="requestToken" sheetId="8" r:id="rId6"/>
+    <sheet name="change-password" sheetId="9" r:id="rId7"/>
+    <sheet name="filters" sheetId="3" r:id="rId8"/>
+    <sheet name="profile" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="401">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1090,6 +1092,156 @@
   </si>
   <si>
     <t>CancelNotifications</t>
+  </si>
+  <si>
+    <t>chooseAccount</t>
+  </si>
+  <si>
+    <t>Choose Account</t>
+  </si>
+  <si>
+    <t>2525150456</t>
+  </si>
+  <si>
+    <t>123487</t>
+  </si>
+  <si>
+    <t>messageToRecipient</t>
+  </si>
+  <si>
+    <t>expColour</t>
+  </si>
+  <si>
+    <t>expRequest</t>
+  </si>
+  <si>
+    <t>expCssProp</t>
+  </si>
+  <si>
+    <t>VerifyRequestToken</t>
+  </si>
+  <si>
+    <t>requestToken</t>
+  </si>
+  <si>
+    <t>76S2CEPODVNGPZHMDJHSHRKNSOFOAXCYXPAOPUATAOVUPGJXKD3A</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>569446a6-aea8-4c4c-ade2-6445c5b07481</t>
+  </si>
+  <si>
+    <t>Hi Hero</t>
+  </si>
+  <si>
+    <t>Tokens Requested Successfully</t>
+  </si>
+  <si>
+    <t>rgb(239, 239, 239)</t>
+  </si>
+  <si>
+    <t>rgb(246, 246, 246)</t>
+  </si>
+  <si>
+    <t>rgb(56,56,56)</t>
+  </si>
+  <si>
+    <t>Verify request token with validations</t>
+  </si>
+  <si>
+    <t>request Token with validation</t>
+  </si>
+  <si>
+    <t>A,@$#</t>
+  </si>
+  <si>
+    <t>H,hahhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhsssssssskadj</t>
+  </si>
+  <si>
+    <t>Verify request token with Invalid Wallet Id</t>
+  </si>
+  <si>
+    <t>Invalid Account Address</t>
+  </si>
+  <si>
+    <t>569446a6-aea8-4c4c-ade2</t>
+  </si>
+  <si>
+    <t>Verify request token with Navigation Option</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>heading1</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>successMsg</t>
+  </si>
+  <si>
+    <t>LandingHeading</t>
+  </si>
+  <si>
+    <t>verify change password</t>
+  </si>
+  <si>
+    <t>verify change password functionality</t>
+  </si>
+  <si>
+    <t>Y5OW7IC3DLTHD2JOVWWH4AEB6QGJPD2ABHTDXTJBJJ2NLX3BZ5VA</t>
+  </si>
+  <si>
+    <t>Verify your identity</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
+    <t>Your Password Was Updated Successfully!</t>
+  </si>
+  <si>
+    <t>Change password with invalid password</t>
+  </si>
+  <si>
+    <t>Please enter your current password</t>
+  </si>
+  <si>
+    <t>Current Password</t>
+  </si>
+  <si>
+    <t>Confirm password is required</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Admin@123123</t>
+  </si>
+  <si>
+    <t>Error: Passwords do not match.</t>
+  </si>
+  <si>
+    <t>Passwords</t>
+  </si>
+  <si>
+    <t>New password should not match with Old password</t>
+  </si>
+  <si>
+    <t>verify change password With invalid Credentials</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1209,6 +1361,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1584,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -5541,10 +5699,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F2C328-44FE-4BE7-9D79-D8AE6FF7329F}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:AI1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5571,7 +5729,7 @@
     <col min="21" max="21" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5638,8 +5796,11 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -5680,8 +5841,11 @@
       <c r="U2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>272</v>
       </c>
@@ -5708,7 +5872,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>272</v>
       </c>
@@ -5738,7 +5902,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -5759,7 +5923,7 @@
         <v>270</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="T5" t="s">
         <v>33</v>
@@ -5768,7 +5932,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>281</v>
       </c>
@@ -5801,7 +5965,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -5834,7 +5998,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -5871,7 +6035,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>292</v>
       </c>
@@ -5894,14 +6058,20 @@
       <c r="O9" t="s">
         <v>294</v>
       </c>
+      <c r="P9" s="5" t="s">
+        <v>271</v>
+      </c>
       <c r="R9" t="s">
         <v>322</v>
       </c>
       <c r="S9" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -5928,7 +6098,7 @@
         <v>75</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>271</v>
+        <v>354</v>
       </c>
       <c r="R10" t="s">
         <v>322</v>
@@ -5943,7 +6113,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>295</v>
       </c>
@@ -5982,7 +6152,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6021,7 +6191,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>295</v>
       </c>
@@ -6063,7 +6233,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P12" r:id="rId1" location="@*&amp;%$" xr:uid="{14652010-8D1C-40AF-904B-7A3CA3C1D17D}"/>
+    <hyperlink ref="P12" r:id="rId1" location="@*&amp;%$" xr:uid="{1F191689-41A3-4184-AFAC-8EAC2F5E8CEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6071,6 +6241,717 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CB4B52-88BF-4AB0-95D7-DE4FB48CEC18}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
+    <col min="2" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="10" width="15" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" customWidth="1"/>
+    <col min="14" max="14" width="21.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="M2" t="s">
+        <v>364</v>
+      </c>
+      <c r="N2" t="s">
+        <v>365</v>
+      </c>
+      <c r="O2" t="s">
+        <v>366</v>
+      </c>
+      <c r="P2" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" t="s">
+        <v>372</v>
+      </c>
+      <c r="N3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="G4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="M4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="M5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{58D49811-C353-46AA-B831-9D185A48799F}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{3BBB91E6-3F52-4B16-96D7-85F933F66919}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{9E3454FB-6873-45D8-97BE-1C047D8DE515}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{C517C301-BA4C-412D-AFD3-64A8F76F4D1F}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{4BE3DF3C-22E2-443A-9A22-D991EB78FDB2}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{4E758F28-1B71-4FD3-903B-2D40166D6428}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{BA4F0F09-CAF9-4C47-9865-305BEF36D246}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{804C1E0A-5CB6-44C3-B96B-B840FBD2DF9B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6D89BB-036C-439B-A4C9-B3C473F79A68}">
+  <dimension ref="A1:U8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.90625" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" customWidth="1"/>
+    <col min="17" max="17" width="15.1796875" customWidth="1"/>
+    <col min="20" max="20" width="11.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="U1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="S2" t="s">
+        <v>390</v>
+      </c>
+      <c r="T2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>387</v>
+      </c>
+      <c r="K3" t="s">
+        <v>388</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" t="s">
+        <v>390</v>
+      </c>
+      <c r="T3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>387</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="P4" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>393</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>387</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="P5" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>395</v>
+      </c>
+      <c r="R5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>387</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="P6" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>398</v>
+      </c>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>387</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="P7" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>393</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>387</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{80C5DBD4-348D-47F2-ACB9-63A356987772}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{5EB4B08F-F375-4A55-82A1-8CFD6A176F24}"/>
+    <hyperlink ref="L2" r:id="rId3" xr:uid="{EB12E087-1636-41DC-8FCE-B8453C7D569E}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{B9CBA747-4BBD-494B-A245-129E046771EC}"/>
+    <hyperlink ref="N2" r:id="rId5" xr:uid="{516AF005-B59A-4AFE-ACE6-76FE6BDCE757}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{0101D0A4-AE2C-449E-A2F4-68B88A9D299D}"/>
+    <hyperlink ref="M4" r:id="rId7" xr:uid="{DEB3960A-5AA6-431C-B5FD-D775320F8242}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{8D789175-4341-491F-AE61-8FFABF5E7753}"/>
+    <hyperlink ref="M5" r:id="rId9" xr:uid="{B34CE74B-3457-41AD-8F13-D039E91510BF}"/>
+    <hyperlink ref="N4" r:id="rId10" xr:uid="{4246BCE2-E1F9-4FBE-97D0-C78A2C81BDC3}"/>
+    <hyperlink ref="M6" r:id="rId11" xr:uid="{BB6D21F5-1EBF-46E1-9610-0723ECDD7C89}"/>
+    <hyperlink ref="N6" r:id="rId12" xr:uid="{CCB87B7D-3179-408F-AE5E-D6F015AF1AEF}"/>
+    <hyperlink ref="D6" r:id="rId13" xr:uid="{4735801E-213C-423B-9B9A-313DE141C3B1}"/>
+    <hyperlink ref="L5" r:id="rId14" xr:uid="{DB8F2D00-3B2B-4E78-8C8F-874F15545D4D}"/>
+    <hyperlink ref="L6" r:id="rId15" xr:uid="{0B2648D0-96E8-4B57-9CB1-2B605FE80FBC}"/>
+    <hyperlink ref="M7" r:id="rId16" xr:uid="{AB66BC3F-EE8B-432A-AB8B-AB52D19454DC}"/>
+    <hyperlink ref="D7" r:id="rId17" xr:uid="{7C397FB8-1E1B-4F99-8FC6-B166803010C3}"/>
+    <hyperlink ref="L7" r:id="rId18" xr:uid="{923D4E30-5297-4C13-8BDC-F89EF96A6C8C}"/>
+    <hyperlink ref="E3" r:id="rId19" xr:uid="{B5AAEB49-76BF-4BA7-929E-7DF0230176B8}"/>
+    <hyperlink ref="D3" r:id="rId20" xr:uid="{8D36914E-88C5-4937-B08C-CC40A466DD5F}"/>
+    <hyperlink ref="L3" r:id="rId21" xr:uid="{05B969DB-FB85-4898-8515-EC8AFEA0C8AC}"/>
+    <hyperlink ref="M3" r:id="rId22" xr:uid="{B18E3AEC-B3D2-47B8-AD9B-25A8CB2CC39F}"/>
+    <hyperlink ref="N3" r:id="rId23" xr:uid="{EFFFAC1E-B0B5-493B-B87C-815686649792}"/>
+    <hyperlink ref="E4:E7" r:id="rId24" display="Admin@999" xr:uid="{E67C0CF9-B157-4AE2-B94F-7ADF70F4E132}"/>
+    <hyperlink ref="D8" r:id="rId25" xr:uid="{08179AE5-32F8-448B-99D3-919E962BA191}"/>
+    <hyperlink ref="E8" r:id="rId26" xr:uid="{D49EF1B4-2FDA-4949-B8D7-ECA893A1D54C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6087,7 +6968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Test Method in Login-Forgot Password.
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (13-12-2-2021)(2)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (15-12-2021)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C32803-362F-412F-AA0C-F206A857A741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280DA2BF-9C4A-4963-A57D-FC5C1189B328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId3"/>
     <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId4"/>
     <sheet name="forgotEmail" sheetId="6" r:id="rId5"/>
-    <sheet name="requestToken" sheetId="8" r:id="rId6"/>
-    <sheet name="change-password" sheetId="9" r:id="rId7"/>
-    <sheet name="filters" sheetId="3" r:id="rId8"/>
-    <sheet name="profile" sheetId="2" r:id="rId9"/>
+    <sheet name="forgotPassword" sheetId="10" r:id="rId6"/>
+    <sheet name="requestToken" sheetId="8" r:id="rId7"/>
+    <sheet name="change-password" sheetId="9" r:id="rId8"/>
+    <sheet name="filters" sheetId="3" r:id="rId9"/>
+    <sheet name="profile" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="433">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1242,6 +1243,102 @@
   </si>
   <si>
     <t>verify change password With invalid Credentials</t>
+  </si>
+  <si>
+    <t>lblEmail</t>
+  </si>
+  <si>
+    <t>CreatePasswordHeading</t>
+  </si>
+  <si>
+    <t>enterPassword</t>
+  </si>
+  <si>
+    <t>successHeading</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>test Forgot Password</t>
+  </si>
+  <si>
+    <t>test Valid Password</t>
+  </si>
+  <si>
+    <t>anudeepg@ideyalabs.com</t>
+  </si>
+  <si>
+    <t>Forgot Password?</t>
+  </si>
+  <si>
+    <t>Create New Password</t>
+  </si>
+  <si>
+    <t>Password Changed</t>
+  </si>
+  <si>
+    <t>Please enter the email address associated with your coyni account below. We will send you a one-time passcode.</t>
+  </si>
+  <si>
+    <t>Test forgot password with invalid Email</t>
+  </si>
+  <si>
+    <t>Test forgot password with empty Email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>addhhf@gmail.com</t>
+  </si>
+  <si>
+    <t>This email is not registered to an account in our system.</t>
+  </si>
+  <si>
+    <t>Test Forgot Password with invalid phone OTP</t>
+  </si>
+  <si>
+    <t>Test Forgot Password with special character and Alphabits</t>
+  </si>
+  <si>
+    <t>@#,asd</t>
+  </si>
+  <si>
+    <t>test Forgot Password with invalid enter and confirm Password</t>
+  </si>
+  <si>
+    <t>test Forgot Password with invalid empty enter Password</t>
+  </si>
+  <si>
+    <t>test Forgot Password with invalid Empty Confirm  Password</t>
+  </si>
+  <si>
+    <t>Please confirm your password</t>
+  </si>
+  <si>
+    <t>test Forgot Password with invalid enter  Password</t>
+  </si>
+  <si>
+    <t>Confirm Password must match with Enter password</t>
+  </si>
+  <si>
+    <t>Admin@1000</t>
+  </si>
+  <si>
+    <t>Password must be at least 8 characters</t>
+  </si>
+  <si>
+    <t>qwedsa</t>
+  </si>
+  <si>
+    <t>Invalid password format. Please try again.</t>
+  </si>
+  <si>
+    <t>asdf12333221</t>
   </si>
 </sst>
 </file>
@@ -1747,25 +1844,25 @@
       <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.36328125" customWidth="1"/>
-    <col min="2" max="2" width="50.08984375" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
-    <col min="6" max="6" width="63.90625" customWidth="1"/>
-    <col min="7" max="7" width="63.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" customWidth="1"/>
+    <col min="7" max="7" width="63.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
-    <col min="10" max="10" width="33.90625" customWidth="1"/>
-    <col min="11" max="11" width="24.6328125" customWidth="1"/>
-    <col min="12" max="12" width="26.453125" customWidth="1"/>
-    <col min="13" max="13" width="32.90625" customWidth="1"/>
-    <col min="14" max="14" width="22.90625" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1830,7 +1927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1859,7 +1956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1889,7 +1986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1919,7 +2016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1948,7 +2045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1980,7 +2077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2009,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2027,7 +2124,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2065,7 +2162,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2097,7 +2194,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2129,7 +2226,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2161,7 +2258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2193,7 +2290,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2216,7 +2313,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2248,7 +2345,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -2277,7 +2374,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2303,7 +2400,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2329,7 +2426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2355,7 +2452,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2395,6 +2492,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:X1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D06DFA-D6F9-4A05-B463-4DDA52F0E3E7}">
   <dimension ref="A1:X21"/>
@@ -2403,18 +2552,18 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2488,7 +2637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -2556,7 +2705,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -2622,7 +2771,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -2687,7 +2836,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -2752,7 +2901,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2817,7 +2966,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -2882,7 +3031,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -2944,7 +3093,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -3006,7 +3155,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -3068,7 +3217,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -3130,7 +3279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -3192,7 +3341,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -3254,7 +3403,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -3316,7 +3465,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -3378,7 +3527,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -3440,7 +3589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -3502,7 +3651,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3567,7 +3716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -3629,7 +3778,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>175</v>
       </c>
@@ -3661,7 +3810,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>177</v>
       </c>
@@ -3785,22 +3934,22 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
-    <col min="6" max="6" width="28.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5703125" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
-    <col min="23" max="23" width="9.54296875" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3874,7 +4023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -3939,7 +4088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -4007,7 +4156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -4072,7 +4221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -4105,7 +4254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -4170,7 +4319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>192</v>
       </c>
@@ -4235,7 +4384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -4309,7 +4458,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -4377,7 +4526,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -4445,7 +4594,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>192</v>
       </c>
@@ -4513,7 +4662,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>192</v>
       </c>
@@ -4581,7 +4730,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>192</v>
       </c>
@@ -4650,7 +4799,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>192</v>
       </c>
@@ -4718,7 +4867,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>192</v>
       </c>
@@ -4786,7 +4935,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -4854,7 +5003,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>192</v>
       </c>
@@ -4922,7 +5071,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -5010,17 +5159,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
-    <col min="6" max="6" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5070,7 +5219,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -5099,7 +5248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -5128,7 +5277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -5157,7 +5306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -5186,7 +5335,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -5206,7 +5355,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>229</v>
       </c>
@@ -5226,7 +5375,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>231</v>
       </c>
@@ -5246,7 +5395,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -5266,7 +5415,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -5286,7 +5435,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>237</v>
       </c>
@@ -5306,7 +5455,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -5326,7 +5475,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -5346,7 +5495,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>243</v>
       </c>
@@ -5366,7 +5515,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -5386,7 +5535,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -5412,7 +5561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>251</v>
       </c>
@@ -5441,7 +5590,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -5470,7 +5619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -5499,7 +5648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -5528,7 +5677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>342</v>
       </c>
@@ -5557,7 +5706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>345</v>
       </c>
@@ -5586,7 +5735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>347</v>
       </c>
@@ -5615,7 +5764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -5701,35 +5850,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F2C328-44FE-4BE7-9D79-D8AE6FF7329F}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.36328125" customWidth="1"/>
-    <col min="2" max="2" width="43.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="65.54296875" customWidth="1"/>
-    <col min="7" max="7" width="43.36328125" customWidth="1"/>
-    <col min="8" max="8" width="21.90625" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="15.08984375" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" customWidth="1"/>
-    <col min="12" max="12" width="15.08984375" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" customWidth="1"/>
-    <col min="14" max="14" width="19.90625" customWidth="1"/>
-    <col min="15" max="15" width="18.453125" customWidth="1"/>
-    <col min="16" max="16" width="12.08984375" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" customWidth="1"/>
-    <col min="20" max="20" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="65.5703125" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5800,7 +5949,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -5845,7 +5994,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>272</v>
       </c>
@@ -5872,7 +6021,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>272</v>
       </c>
@@ -5902,7 +6051,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -5932,7 +6081,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>281</v>
       </c>
@@ -5965,7 +6114,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -5998,7 +6147,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -6035,7 +6184,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>292</v>
       </c>
@@ -6071,7 +6220,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -6113,7 +6262,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>295</v>
       </c>
@@ -6152,7 +6301,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6191,7 +6340,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>295</v>
       </c>
@@ -6241,6 +6390,522 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8A0C5-E174-4C21-930E-B9BC756C35D5}">
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>412</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>409</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>416</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>409</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" t="s">
+        <v>418</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>409</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>419</v>
+      </c>
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>409</v>
+      </c>
+      <c r="H6" t="s">
+        <v>294</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>420</v>
+      </c>
+      <c r="B7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>409</v>
+      </c>
+      <c r="H7" t="s">
+        <v>294</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>409</v>
+      </c>
+      <c r="H8" t="s">
+        <v>294</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K8" t="s">
+        <v>410</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E9" t="s">
+        <v>425</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>409</v>
+      </c>
+      <c r="H9" t="s">
+        <v>294</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K9" t="s">
+        <v>410</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>422</v>
+      </c>
+      <c r="B10" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E10" t="s">
+        <v>427</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>409</v>
+      </c>
+      <c r="H10" t="s">
+        <v>294</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K10" t="s">
+        <v>410</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>422</v>
+      </c>
+      <c r="B11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E11" t="s">
+        <v>429</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>409</v>
+      </c>
+      <c r="H11" t="s">
+        <v>294</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K11" t="s">
+        <v>410</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B12" t="s">
+        <v>426</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E12" t="s">
+        <v>431</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>409</v>
+      </c>
+      <c r="H12" t="s">
+        <v>294</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K12" t="s">
+        <v>410</v>
+      </c>
+      <c r="L12" t="s">
+        <v>432</v>
+      </c>
+      <c r="M12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{C5FAF50F-DF40-4AE3-B797-DE228EDFBB1F}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{67ABC54D-C962-4462-A3E0-826AE42448D8}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{C9CCF2A7-CF36-432E-890A-A7BCA1FF47B9}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{DD61AAFD-F0FD-4B0D-B4F3-F891C829242B}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{03FE81E9-1EFD-43FC-AEBC-38AF16682ED8}"/>
+    <hyperlink ref="I6" r:id="rId6" xr:uid="{1C962E9C-AFC7-4C22-8EDB-05EE9E74433E}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{D6D3DC59-640D-4095-A43B-E7A35CBF0BD9}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{618777BA-2773-4087-940E-4B93335C6229}"/>
+    <hyperlink ref="I7" r:id="rId9" xr:uid="{E93FD0E8-4D4F-422B-8185-273EF680331A}"/>
+    <hyperlink ref="I8" r:id="rId10" xr:uid="{66B297C9-743A-42CB-B994-9B6ABCB5090E}"/>
+    <hyperlink ref="M8" r:id="rId11" xr:uid="{D730F95F-1B02-4C44-A6CD-8C81808B9EF3}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{E0AA9C3F-A871-4A13-8920-5921B29B7D38}"/>
+    <hyperlink ref="I9" r:id="rId13" xr:uid="{56709C27-797F-4B60-9975-06CA347065E9}"/>
+    <hyperlink ref="L9" r:id="rId14" xr:uid="{EA36490E-DAEE-456D-95B3-18E3BA2FC2AC}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{CA13EF44-A3FD-4723-B2A4-44564B6A4CB7}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{44596E6E-7A0F-4499-AC8A-B0D01D875FB1}"/>
+    <hyperlink ref="I10" r:id="rId17" xr:uid="{F1304E7E-E453-4445-8CE4-EB556AED58B3}"/>
+    <hyperlink ref="L10" r:id="rId18" display="Admin@999" xr:uid="{34CA6E72-9F8E-45FF-BE12-2C1FEC02B52B}"/>
+    <hyperlink ref="M10" r:id="rId19" xr:uid="{999D8EDE-EF24-439B-AC9A-07A97FD76C16}"/>
+    <hyperlink ref="D11" r:id="rId20" xr:uid="{5546C8FF-DDE4-4699-A9DB-8B9C33921BC1}"/>
+    <hyperlink ref="I11" r:id="rId21" xr:uid="{991895A0-ABA4-4785-9CE4-62587659BF8F}"/>
+    <hyperlink ref="D12" r:id="rId22" xr:uid="{B2852A54-FD2C-4AFE-A0F4-74485806F686}"/>
+    <hyperlink ref="I12" r:id="rId23" xr:uid="{4BCBE6FB-0C1F-4266-81EB-902B68678C01}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CB4B52-88BF-4AB0-95D7-DE4FB48CEC18}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -6248,19 +6913,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
     <col min="8" max="10" width="15" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
-    <col min="13" max="13" width="18.81640625" customWidth="1"/>
-    <col min="14" max="14" width="21.26953125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6313,7 +6978,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>359</v>
       </c>
@@ -6363,7 +7028,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>369</v>
       </c>
@@ -6402,7 +7067,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>373</v>
       </c>
@@ -6443,7 +7108,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>376</v>
       </c>
@@ -6496,7 +7161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6D89BB-036C-439B-A4C9-B3C473F79A68}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -6504,29 +7169,29 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.453125" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="19.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" customWidth="1"/>
-    <col min="10" max="10" width="20.54296875" customWidth="1"/>
-    <col min="11" max="11" width="16.90625" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" customWidth="1"/>
-    <col min="17" max="17" width="15.1796875" customWidth="1"/>
-    <col min="20" max="20" width="11.6328125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6589,7 +7254,7 @@
       </c>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>384</v>
       </c>
@@ -6640,7 +7305,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>384</v>
       </c>
@@ -6690,7 +7355,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>391</v>
       </c>
@@ -6737,7 +7402,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>391</v>
       </c>
@@ -6785,7 +7450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>391</v>
       </c>
@@ -6835,7 +7500,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>391</v>
       </c>
@@ -6883,7 +7548,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>400</v>
       </c>
@@ -6951,7 +7616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6961,61 +7626,9 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:X1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.36328125" customWidth="1"/>
-    <col min="6" max="6" width="30.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test methods in Forgot Email
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (15-12-2021)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (29-12-2021)[2]\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280DA2BF-9C4A-4963-A57D-FC5C1189B328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8357F0-069F-4D6D-8394-D0816B999B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="401">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1243,102 +1243,6 @@
   </si>
   <si>
     <t>verify change password With invalid Credentials</t>
-  </si>
-  <si>
-    <t>lblEmail</t>
-  </si>
-  <si>
-    <t>CreatePasswordHeading</t>
-  </si>
-  <si>
-    <t>enterPassword</t>
-  </si>
-  <si>
-    <t>successHeading</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>test Forgot Password</t>
-  </si>
-  <si>
-    <t>test Valid Password</t>
-  </si>
-  <si>
-    <t>anudeepg@ideyalabs.com</t>
-  </si>
-  <si>
-    <t>Forgot Password?</t>
-  </si>
-  <si>
-    <t>Create New Password</t>
-  </si>
-  <si>
-    <t>Password Changed</t>
-  </si>
-  <si>
-    <t>Please enter the email address associated with your coyni account below. We will send you a one-time passcode.</t>
-  </si>
-  <si>
-    <t>Test forgot password with invalid Email</t>
-  </si>
-  <si>
-    <t>Test forgot password with empty Email</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>addhhf@gmail.com</t>
-  </si>
-  <si>
-    <t>This email is not registered to an account in our system.</t>
-  </si>
-  <si>
-    <t>Test Forgot Password with invalid phone OTP</t>
-  </si>
-  <si>
-    <t>Test Forgot Password with special character and Alphabits</t>
-  </si>
-  <si>
-    <t>@#,asd</t>
-  </si>
-  <si>
-    <t>test Forgot Password with invalid enter and confirm Password</t>
-  </si>
-  <si>
-    <t>test Forgot Password with invalid empty enter Password</t>
-  </si>
-  <si>
-    <t>test Forgot Password with invalid Empty Confirm  Password</t>
-  </si>
-  <si>
-    <t>Please confirm your password</t>
-  </si>
-  <si>
-    <t>test Forgot Password with invalid enter  Password</t>
-  </si>
-  <si>
-    <t>Confirm Password must match with Enter password</t>
-  </si>
-  <si>
-    <t>Admin@1000</t>
-  </si>
-  <si>
-    <t>Password must be at least 8 characters</t>
-  </si>
-  <si>
-    <t>qwedsa</t>
-  </si>
-  <si>
-    <t>Invalid password format. Please try again.</t>
-  </si>
-  <si>
-    <t>asdf12333221</t>
   </si>
 </sst>
 </file>
@@ -1844,25 +1748,25 @@
       <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="63.85546875" customWidth="1"/>
-    <col min="7" max="7" width="63.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="63.81640625" customWidth="1"/>
+    <col min="7" max="7" width="63.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" customWidth="1"/>
-    <col min="13" max="13" width="32.85546875" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.81640625" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="26.453125" customWidth="1"/>
+    <col min="13" max="13" width="32.81640625" customWidth="1"/>
+    <col min="14" max="14" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +1831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1956,7 +1860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1986,7 +1890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +1920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2045,7 +1949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2077,7 +1981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2106,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2028,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2162,7 +2066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2194,7 +2098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2226,7 +2130,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2258,7 +2162,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2290,7 +2194,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2313,7 +2217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2345,7 +2249,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -2374,7 +2278,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2400,7 +2304,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2426,7 +2330,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2452,7 +2356,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2500,16 +2404,16 @@
       <selection activeCell="J1" sqref="J1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2552,18 +2456,18 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -2705,7 +2609,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -2771,7 +2675,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -2836,7 +2740,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -2901,7 +2805,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2966,7 +2870,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -3031,7 +2935,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -3093,7 +2997,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -3155,7 +3059,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -3217,7 +3121,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -3279,7 +3183,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -3341,7 +3245,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -3403,7 +3307,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -3465,7 +3369,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -3527,7 +3431,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -3589,7 +3493,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -3651,7 +3555,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3716,7 +3620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -3778,7 +3682,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>175</v>
       </c>
@@ -3810,7 +3714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>177</v>
       </c>
@@ -3934,22 +3838,22 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.54296875" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +3927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -4088,7 +3992,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -4156,7 +4060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -4221,7 +4125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -4254,7 +4158,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -4319,7 +4223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>192</v>
       </c>
@@ -4384,7 +4288,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -4458,7 +4362,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -4526,7 +4430,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -4594,7 +4498,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>192</v>
       </c>
@@ -4662,7 +4566,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>192</v>
       </c>
@@ -4730,7 +4634,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>192</v>
       </c>
@@ -4799,7 +4703,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>192</v>
       </c>
@@ -4867,7 +4771,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>192</v>
       </c>
@@ -4935,7 +4839,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -5003,7 +4907,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>192</v>
       </c>
@@ -5071,7 +4975,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -5159,17 +5063,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5219,7 +5123,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -5248,7 +5152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -5277,7 +5181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -5306,7 +5210,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -5335,7 +5239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -5355,7 +5259,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>229</v>
       </c>
@@ -5375,7 +5279,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>231</v>
       </c>
@@ -5395,7 +5299,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -5415,7 +5319,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -5435,7 +5339,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>237</v>
       </c>
@@ -5455,7 +5359,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -5475,7 +5379,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -5495,7 +5399,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>243</v>
       </c>
@@ -5515,7 +5419,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -5535,7 +5439,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -5561,7 +5465,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>251</v>
       </c>
@@ -5590,7 +5494,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -5619,7 +5523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -5648,7 +5552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -5677,7 +5581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>342</v>
       </c>
@@ -5706,7 +5610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>345</v>
       </c>
@@ -5735,7 +5639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>347</v>
       </c>
@@ -5764,7 +5668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -5854,31 +5758,31 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="65.5703125" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="65.54296875" customWidth="1"/>
+    <col min="7" max="7" width="43.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" customWidth="1"/>
+    <col min="11" max="11" width="20.453125" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="19.81640625" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" customWidth="1"/>
+    <col min="20" max="20" width="16.54296875" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5949,7 +5853,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>268</v>
       </c>
@@ -5994,7 +5898,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>272</v>
       </c>
@@ -6021,7 +5925,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>272</v>
       </c>
@@ -6051,7 +5955,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -6081,7 +5985,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>281</v>
       </c>
@@ -6114,7 +6018,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -6147,7 +6051,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -6184,7 +6088,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>292</v>
       </c>
@@ -6220,7 +6124,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>295</v>
       </c>
@@ -6262,7 +6166,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>295</v>
       </c>
@@ -6301,7 +6205,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>295</v>
       </c>
@@ -6340,7 +6244,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>295</v>
       </c>
@@ -6391,31 +6295,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8A0C5-E174-4C21-930E-B9BC756C35D5}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="52.1796875" customWidth="1"/>
+    <col min="2" max="2" width="46.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="21.54296875" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" customWidth="1"/>
+    <col min="14" max="14" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6429,478 +6333,498 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
-        <v>407</v>
+        <v>269</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="G2" t="s">
-        <v>409</v>
-      </c>
-      <c r="H2" t="s">
-        <v>294</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="L2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2525150178</v>
+      </c>
+      <c r="O2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="K2" t="s">
-        <v>410</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>412</v>
-      </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>322</v>
       </c>
       <c r="S2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="T2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
+        <v>324</v>
+      </c>
+      <c r="W2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>273</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" t="s">
-        <v>409</v>
-      </c>
-      <c r="O3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>270</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="P3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
-        <v>413</v>
+        <v>276</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>416</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" t="s">
-        <v>409</v>
-      </c>
-      <c r="O4" t="s">
+        <v>277</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>270</v>
+      </c>
+      <c r="M4">
+        <v>9515</v>
+      </c>
+      <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="P4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>413</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s">
-        <v>413</v>
+        <v>279</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E5" t="s">
-        <v>418</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="G5" t="s">
-        <v>409</v>
-      </c>
-      <c r="O5" t="s">
+        <v>280</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>270</v>
+      </c>
+      <c r="M5">
+        <v>2525150456</v>
+      </c>
+      <c r="T5" t="s">
         <v>33</v>
       </c>
-      <c r="P5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>419</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>282</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2"/>
+      <c r="G6" t="s">
+        <v>283</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="L6" t="s">
+        <v>270</v>
+      </c>
+      <c r="M6">
+        <v>2525150178</v>
+      </c>
+      <c r="S6" t="s">
+        <v>323</v>
+      </c>
+      <c r="T6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="G7" t="s">
+        <v>286</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="L7" t="s">
+        <v>270</v>
+      </c>
+      <c r="M7">
+        <v>2525150178</v>
+      </c>
+      <c r="R7" t="s">
+        <v>322</v>
+      </c>
+      <c r="T7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="L8" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2525150178</v>
+      </c>
+      <c r="R8" t="s">
+        <v>289</v>
+      </c>
+      <c r="S8" t="s">
+        <v>290</v>
+      </c>
+      <c r="T8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="L9" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M9">
+        <v>2525150178</v>
+      </c>
+      <c r="O9" t="s">
+        <v>294</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="R9" t="s">
+        <v>322</v>
+      </c>
+      <c r="S9" t="s">
+        <v>323</v>
+      </c>
+      <c r="W9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="G10" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>409</v>
-      </c>
-      <c r="H6" t="s">
-        <v>294</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="I10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="L10" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2525150178</v>
+      </c>
+      <c r="O10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R10" t="s">
+        <v>322</v>
+      </c>
+      <c r="S10" t="s">
+        <v>323</v>
+      </c>
+      <c r="T10" t="s">
         <v>33</v>
       </c>
-      <c r="P6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>420</v>
-      </c>
-      <c r="B7" t="s">
-        <v>420</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>409</v>
-      </c>
-      <c r="H7" t="s">
-        <v>294</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>422</v>
-      </c>
-      <c r="B8" t="s">
-        <v>423</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>409</v>
-      </c>
-      <c r="H8" t="s">
-        <v>294</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K8" t="s">
-        <v>410</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>422</v>
-      </c>
-      <c r="B9" t="s">
-        <v>424</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="U10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E9" t="s">
-        <v>425</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>409</v>
-      </c>
-      <c r="H9" t="s">
-        <v>294</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K9" t="s">
-        <v>410</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="D11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="L11" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M11" s="2">
+        <v>2525150178</v>
+      </c>
+      <c r="O11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" t="s">
+        <v>297</v>
+      </c>
+      <c r="R11" t="s">
+        <v>322</v>
+      </c>
+      <c r="S11" t="s">
+        <v>323</v>
+      </c>
+      <c r="T11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E10" t="s">
-        <v>427</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>409</v>
-      </c>
-      <c r="H10" t="s">
-        <v>294</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K10" t="s">
-        <v>410</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>422</v>
-      </c>
-      <c r="B11" t="s">
-        <v>426</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="L12" t="s">
+        <v>270</v>
+      </c>
+      <c r="M12">
+        <v>2525150178</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" t="s">
+        <v>298</v>
+      </c>
+      <c r="R12" t="s">
+        <v>322</v>
+      </c>
+      <c r="S12" t="s">
+        <v>323</v>
+      </c>
+      <c r="T12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E11" t="s">
-        <v>429</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>409</v>
-      </c>
-      <c r="H11" t="s">
-        <v>294</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K11" t="s">
-        <v>410</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>422</v>
-      </c>
-      <c r="B12" t="s">
-        <v>426</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E12" t="s">
-        <v>431</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>409</v>
-      </c>
-      <c r="H12" t="s">
-        <v>294</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K12" t="s">
-        <v>410</v>
-      </c>
-      <c r="L12" t="s">
-        <v>432</v>
-      </c>
-      <c r="M12" t="s">
-        <v>432</v>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>270</v>
+      </c>
+      <c r="M13">
+        <v>2525150178</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" t="s">
+        <v>299</v>
+      </c>
+      <c r="R13" t="s">
+        <v>322</v>
+      </c>
+      <c r="S13" t="s">
+        <v>323</v>
+      </c>
+      <c r="T13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{C5FAF50F-DF40-4AE3-B797-DE228EDFBB1F}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{67ABC54D-C962-4462-A3E0-826AE42448D8}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{C9CCF2A7-CF36-432E-890A-A7BCA1FF47B9}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{DD61AAFD-F0FD-4B0D-B4F3-F891C829242B}"/>
-    <hyperlink ref="D5" r:id="rId5" xr:uid="{03FE81E9-1EFD-43FC-AEBC-38AF16682ED8}"/>
-    <hyperlink ref="I6" r:id="rId6" xr:uid="{1C962E9C-AFC7-4C22-8EDB-05EE9E74433E}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{D6D3DC59-640D-4095-A43B-E7A35CBF0BD9}"/>
-    <hyperlink ref="D7" r:id="rId8" xr:uid="{618777BA-2773-4087-940E-4B93335C6229}"/>
-    <hyperlink ref="I7" r:id="rId9" xr:uid="{E93FD0E8-4D4F-422B-8185-273EF680331A}"/>
-    <hyperlink ref="I8" r:id="rId10" xr:uid="{66B297C9-743A-42CB-B994-9B6ABCB5090E}"/>
-    <hyperlink ref="M8" r:id="rId11" xr:uid="{D730F95F-1B02-4C44-A6CD-8C81808B9EF3}"/>
-    <hyperlink ref="D8" r:id="rId12" xr:uid="{E0AA9C3F-A871-4A13-8920-5921B29B7D38}"/>
-    <hyperlink ref="I9" r:id="rId13" xr:uid="{56709C27-797F-4B60-9975-06CA347065E9}"/>
-    <hyperlink ref="L9" r:id="rId14" xr:uid="{EA36490E-DAEE-456D-95B3-18E3BA2FC2AC}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{CA13EF44-A3FD-4723-B2A4-44564B6A4CB7}"/>
-    <hyperlink ref="D10" r:id="rId16" xr:uid="{44596E6E-7A0F-4499-AC8A-B0D01D875FB1}"/>
-    <hyperlink ref="I10" r:id="rId17" xr:uid="{F1304E7E-E453-4445-8CE4-EB556AED58B3}"/>
-    <hyperlink ref="L10" r:id="rId18" display="Admin@999" xr:uid="{34CA6E72-9F8E-45FF-BE12-2C1FEC02B52B}"/>
-    <hyperlink ref="M10" r:id="rId19" xr:uid="{999D8EDE-EF24-439B-AC9A-07A97FD76C16}"/>
-    <hyperlink ref="D11" r:id="rId20" xr:uid="{5546C8FF-DDE4-4699-A9DB-8B9C33921BC1}"/>
-    <hyperlink ref="I11" r:id="rId21" xr:uid="{991895A0-ABA4-4785-9CE4-62587659BF8F}"/>
-    <hyperlink ref="D12" r:id="rId22" xr:uid="{B2852A54-FD2C-4AFE-A0F4-74485806F686}"/>
-    <hyperlink ref="I12" r:id="rId23" xr:uid="{4BCBE6FB-0C1F-4266-81EB-902B68678C01}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6913,19 +6837,19 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
     <col min="2" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
     <col min="8" max="10" width="15" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" customWidth="1"/>
+    <col min="14" max="14" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6978,7 +6902,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>359</v>
       </c>
@@ -7028,7 +6952,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>369</v>
       </c>
@@ -7067,7 +6991,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>373</v>
       </c>
@@ -7108,7 +7032,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>376</v>
       </c>
@@ -7169,29 +7093,29 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" customWidth="1"/>
+    <col min="17" max="17" width="15.1796875" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7254,7 +7178,7 @@
       </c>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>384</v>
       </c>
@@ -7305,7 +7229,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>384</v>
       </c>
@@ -7355,7 +7279,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>391</v>
       </c>
@@ -7402,7 +7326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>391</v>
       </c>
@@ -7450,7 +7374,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>391</v>
       </c>
@@ -7500,7 +7424,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>391</v>
       </c>
@@ -7548,7 +7472,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>400</v>
       </c>
@@ -7626,7 +7550,7 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test script in NavigationTest
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (29-12-2021)[2]\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (05-01-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8357F0-069F-4D6D-8394-D0816B999B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D337ED-360F-4556-90E8-1F8117C5F50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="427">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1243,6 +1243,84 @@
   </si>
   <si>
     <t>verify change password With invalid Credentials</t>
+  </si>
+  <si>
+    <t>Verify My QR code With Email</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>gubbaanudeep@yahoo.com</t>
+  </si>
+  <si>
+    <t>UYL3VUUWNJ7CTBIGUZXZKAOAWYYTCTKBQUMF2XXID7CWXOHIXVDA</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Copied to clipboard</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Verify My QR code with Navigation Option</t>
+  </si>
+  <si>
+    <t>QR Code with navigation option</t>
+  </si>
+  <si>
+    <t>Verify My QR code with Paste Option</t>
+  </si>
+  <si>
+    <t>QR Code with paste option</t>
+  </si>
+  <si>
+    <t>Verify My QR code With Phone Number</t>
+  </si>
+  <si>
+    <t>Verify My QR code With nagative option</t>
+  </si>
+  <si>
+    <t>Empty Email</t>
+  </si>
+  <si>
+    <t>please enter Email</t>
+  </si>
+  <si>
+    <t>invalid Email</t>
+  </si>
+  <si>
+    <t>dsdf</t>
+  </si>
+  <si>
+    <t>Empty Phone Number</t>
+  </si>
+  <si>
+    <t>please enter Phone Number</t>
+  </si>
+  <si>
+    <t>invalid Phone Number</t>
+  </si>
+  <si>
+    <t>Phone number must be10 digits</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>copyToClipBoard</t>
+  </si>
+  <si>
+    <t>containt</t>
+  </si>
+  <si>
+    <t>email1</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
@@ -5057,10 +5135,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7342C061-16F1-49A5-BA07-4D17E62E882D}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5068,12 +5146,12 @@
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="31.54296875" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" customWidth="1"/>
     <col min="6" max="6" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5122,8 +5200,26 @@
       <c r="P1" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -5152,7 +5248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -5181,7 +5277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -5210,7 +5306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -5239,7 +5335,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -5259,7 +5355,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>229</v>
       </c>
@@ -5279,7 +5375,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>231</v>
       </c>
@@ -5299,7 +5395,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -5319,7 +5415,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -5339,7 +5435,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>237</v>
       </c>
@@ -5359,7 +5455,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>239</v>
       </c>
@@ -5379,7 +5475,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -5399,7 +5495,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>243</v>
       </c>
@@ -5419,7 +5515,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -5439,7 +5535,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -5465,7 +5561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>251</v>
       </c>
@@ -5494,7 +5590,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -5523,7 +5619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -5552,7 +5648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -5581,7 +5677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>342</v>
       </c>
@@ -5610,7 +5706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>345</v>
       </c>
@@ -5639,7 +5735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>347</v>
       </c>
@@ -5668,7 +5764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -5697,18 +5793,313 @@
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>401</v>
+      </c>
+      <c r="B25" t="s">
+        <v>402</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>404</v>
+      </c>
+      <c r="L25" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>405</v>
+      </c>
+      <c r="R25" t="s">
+        <v>406</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="T25" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>408</v>
+      </c>
+      <c r="B26" t="s">
+        <v>409</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>404</v>
+      </c>
+      <c r="L26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" t="s">
+        <v>29</v>
+      </c>
+      <c r="S26" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="T26" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>410</v>
+      </c>
+      <c r="B27" t="s">
+        <v>411</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>404</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>412</v>
+      </c>
+      <c r="B28" t="s">
+        <v>402</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>404</v>
+      </c>
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>405</v>
+      </c>
+      <c r="R28" t="s">
+        <v>406</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="T28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>413</v>
+      </c>
+      <c r="B29" t="s">
+        <v>414</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>404</v>
+      </c>
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" t="s">
+        <v>29</v>
+      </c>
+      <c r="R29" t="s">
+        <v>406</v>
+      </c>
+      <c r="U29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>413</v>
+      </c>
+      <c r="B30" t="s">
+        <v>416</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>404</v>
+      </c>
+      <c r="L30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>29</v>
+      </c>
+      <c r="R30" t="s">
+        <v>406</v>
+      </c>
+      <c r="U30" t="s">
+        <v>40</v>
+      </c>
+      <c r="V30" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>413</v>
+      </c>
+      <c r="B31" t="s">
+        <v>418</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>404</v>
+      </c>
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" t="s">
+        <v>29</v>
+      </c>
+      <c r="R31" t="s">
+        <v>406</v>
+      </c>
+      <c r="U31" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B32" t="s">
+        <v>420</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>404</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" t="s">
+        <v>406</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="U32" t="s">
+        <v>421</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{6C146171-EEEB-4984-BA7E-C72A2C6B51F4}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{59FF07A1-4463-4523-9767-833F2DE70D1C}"/>
-    <hyperlink ref="E21" r:id="rId3" xr:uid="{DFEEEE0B-B654-4EA9-9E5F-A2ECC164D06F}"/>
-    <hyperlink ref="E22" r:id="rId4" xr:uid="{FDCC25EC-5380-48E3-8E76-81356C607A09}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{C71CD914-5C7B-4719-883C-7618E52BE817}"/>
-    <hyperlink ref="D21" r:id="rId6" xr:uid="{1FD25F7D-AAB5-4BAA-ADF8-5583B4A7AE7B}"/>
-    <hyperlink ref="D22" r:id="rId7" xr:uid="{4B0EF301-F251-4899-A408-95EB86321974}"/>
-    <hyperlink ref="D23" r:id="rId8" xr:uid="{86C448C7-75C2-4C71-AB76-254382979C63}"/>
-    <hyperlink ref="E24" r:id="rId9" xr:uid="{24CC7C77-505F-44A5-A8B6-654B4141B30D}"/>
-    <hyperlink ref="D24" r:id="rId10" xr:uid="{F5C5EC36-8809-432B-897D-458331D1C6C1}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{DFEEEE0B-B654-4EA9-9E5F-A2ECC164D06F}"/>
+    <hyperlink ref="E22" r:id="rId2" xr:uid="{FDCC25EC-5380-48E3-8E76-81356C607A09}"/>
+    <hyperlink ref="E23" r:id="rId3" xr:uid="{C71CD914-5C7B-4719-883C-7618E52BE817}"/>
+    <hyperlink ref="D21" r:id="rId4" xr:uid="{1FD25F7D-AAB5-4BAA-ADF8-5583B4A7AE7B}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{4B0EF301-F251-4899-A408-95EB86321974}"/>
+    <hyperlink ref="D23" r:id="rId6" xr:uid="{86C448C7-75C2-4C71-AB76-254382979C63}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{24CC7C77-505F-44A5-A8B6-654B4141B30D}"/>
+    <hyperlink ref="D24" r:id="rId8" xr:uid="{F5C5EC36-8809-432B-897D-458331D1C6C1}"/>
+    <hyperlink ref="D2" r:id="rId9" xr:uid="{6C146171-EEEB-4984-BA7E-C72A2C6B51F4}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{59FF07A1-4463-4523-9767-833F2DE70D1C}"/>
     <hyperlink ref="E3" r:id="rId11" xr:uid="{9A98EE61-435E-4D38-8B59-1074A85B2EA7}"/>
     <hyperlink ref="E4" r:id="rId12" xr:uid="{46E5BC6B-E5B6-41EE-B95C-F7A8228F3D09}"/>
     <hyperlink ref="E5" r:id="rId13" xr:uid="{6CE74440-7463-4E39-BB8F-EB4E280D5C96}"/>
@@ -5745,6 +6136,9 @@
     <hyperlink ref="D18" r:id="rId44" xr:uid="{8DEFF7FE-2426-47DD-ADA5-319A052EE5AB}"/>
     <hyperlink ref="D19" r:id="rId45" xr:uid="{49E10451-CE4B-4673-B443-EC5C0A0CF61A}"/>
     <hyperlink ref="D20" r:id="rId46" xr:uid="{3BB0A350-CFD3-44D8-B3F3-D435CB0295DF}"/>
+    <hyperlink ref="E25:E32" r:id="rId47" display="Cust@123" xr:uid="{A6412B37-8416-4F86-9F23-3E465150F710}"/>
+    <hyperlink ref="D25" r:id="rId48" xr:uid="{9D48A650-565B-4079-A94C-14CF4D657E9F}"/>
+    <hyperlink ref="D26:D32" r:id="rId49" display="gubbaanudeep@yahoo.com" xr:uid="{D3F1C163-E43C-4ABE-860D-3F8FD5505935}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6297,7 +6691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8A0C5-E174-4C21-930E-B9BC756C35D5}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Test Script for Change password
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpace-08-01-2022\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (17-01-2021)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140449AC-7D8C-4F12-A411-9E67D6D5C172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328122F1-30D0-42C8-A15E-E1383AE882AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="User-Details" sheetId="10" r:id="rId2"/>
-    <sheet name="PaymentMethods" sheetId="4" r:id="rId3"/>
-    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId4"/>
-    <sheet name="forgotEmail" sheetId="6" r:id="rId5"/>
-    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId6"/>
-    <sheet name="filters" sheetId="3" r:id="rId7"/>
-    <sheet name="profile" sheetId="2" r:id="rId8"/>
-    <sheet name="homePage" sheetId="9" r:id="rId9"/>
+    <sheet name="changePassword" sheetId="11" r:id="rId3"/>
+    <sheet name="PaymentMethods" sheetId="4" r:id="rId4"/>
+    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId5"/>
+    <sheet name="forgotEmail" sheetId="6" r:id="rId6"/>
+    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId7"/>
+    <sheet name="filters" sheetId="3" r:id="rId8"/>
+    <sheet name="profile" sheetId="2" r:id="rId9"/>
+    <sheet name="homePage" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2266" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="578">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1709,13 +1710,82 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>successContent</t>
+  </si>
+  <si>
+    <t>createHeading</t>
+  </si>
+  <si>
+    <t>test Change Password</t>
+  </si>
+  <si>
+    <t>valid change password</t>
+  </si>
+  <si>
+    <t>maniv789396@gmail.com</t>
+  </si>
+  <si>
+    <t>IABM32UV4QPB7LGO7HEWRQM4CFU2KA2BDZ473FYHLEPEXC4QRT6A</t>
+  </si>
+  <si>
+    <t>Verify your Identity</t>
+  </si>
+  <si>
+    <t>As a security measure, you will be logged out of your
+account once you successfully change your password.</t>
+  </si>
+  <si>
+    <t>Your Password Was Updated Successfully!</t>
+  </si>
+  <si>
+    <t>test Change Password ivalid information</t>
+  </si>
+  <si>
+    <t>invalid confirm password</t>
+  </si>
+  <si>
+    <t>Admin@1234</t>
+  </si>
+  <si>
+    <t>Admin@1235</t>
+  </si>
+  <si>
+    <t>Error: Passwords do not match.</t>
+  </si>
+  <si>
+    <t>empty confirm password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Confirm password is required
+</t>
+  </si>
+  <si>
+    <t>empty current password</t>
+  </si>
+  <si>
+    <t>Password is required</t>
+  </si>
+  <si>
+    <t>New password should not match with Old password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1810,6 +1880,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1848,7 +1924,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1908,6 +1984,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2289,25 +2368,25 @@
       <selection pane="topRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="63.88671875" customWidth="1"/>
-    <col min="7" max="7" width="63.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.453125" customWidth="1"/>
+    <col min="2" max="2" width="50.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="27.08984375" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="63.90625" customWidth="1"/>
+    <col min="7" max="7" width="63.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
-    <col min="10" max="10" width="33.88671875" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.44140625" customWidth="1"/>
-    <col min="13" max="13" width="32.88671875" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="33.90625" customWidth="1"/>
+    <col min="11" max="11" width="24.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.453125" customWidth="1"/>
+    <col min="13" max="13" width="32.90625" customWidth="1"/>
+    <col min="14" max="14" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2401,7 +2480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2431,7 +2510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2461,7 +2540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2490,7 +2569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2522,7 +2601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2551,7 +2630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2569,7 +2648,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2607,7 +2686,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2639,7 +2718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2671,7 +2750,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2703,7 +2782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2735,7 +2814,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2758,7 +2837,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2790,7 +2869,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -2819,7 +2898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2845,7 +2924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2871,7 +2950,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2897,7 +2976,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -2939,40 +3018,1016 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B18C423-D7E7-4B7B-9167-D2BDC190AA4E}">
+  <dimension ref="A1:W22"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.453125" customWidth="1"/>
+    <col min="2" max="2" width="48.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="24.90625" customWidth="1"/>
+    <col min="5" max="5" width="35.90625" customWidth="1"/>
+    <col min="6" max="6" width="35.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="9" max="9" width="49.08984375" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" customWidth="1"/>
+    <col min="15" max="15" width="19.36328125" customWidth="1"/>
+    <col min="16" max="16" width="23.6328125" customWidth="1"/>
+    <col min="17" max="18" width="19.36328125" customWidth="1"/>
+    <col min="19" max="19" width="22.6328125" customWidth="1"/>
+    <col min="20" max="20" width="19.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+    </row>
+    <row r="3" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>405</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="K3" s="16"/>
+      <c r="L3" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="I4" t="s">
+        <v>442</v>
+      </c>
+      <c r="J4" t="s">
+        <v>442</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" t="s">
+        <v>456</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J7" t="s">
+        <v>456</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="V7" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" t="s">
+        <v>476</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="I8" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J8" t="s">
+        <v>456</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J9" t="s">
+        <v>456</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="V9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B10" t="s">
+        <v>480</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>481</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J10" t="s">
+        <v>456</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" t="s">
+        <v>482</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
+        <v>483</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J11" t="s">
+        <v>456</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U11" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" t="s">
+        <v>485</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J12" t="s">
+        <v>456</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U12" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B13" t="s">
+        <v>487</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J13" t="s">
+        <v>456</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U13" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B14" t="s">
+        <v>489</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J14" t="s">
+        <v>456</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="V14" t="s">
+        <v>49</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15" t="s">
+        <v>491</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>492</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="F15" s="20"/>
+      <c r="I15" s="19"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U15" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B16" t="s">
+        <v>493</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J16" t="s">
+        <v>456</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U16" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J17" t="s">
+        <v>456</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="U17" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" t="s">
+        <v>496</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>497</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J18" t="s">
+        <v>456</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B19" t="s">
+        <v>499</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J19" t="s">
+        <v>456</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B20" t="s">
+        <v>501</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J20" t="s">
+        <v>456</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B21" t="s">
+        <v>502</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J21" t="s">
+        <v>456</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B22" t="s">
+        <v>504</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{40B15EDC-AE23-443B-B49A-CCCCBA695541}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{34364467-99E6-4A73-9F0A-367BEB8795A2}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{76ED8F48-D6F5-4471-9E0F-F1693D3E4241}"/>
+    <hyperlink ref="D4" r:id="rId4" display="a@b.in,a@b.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghiklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefgdhijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com" xr:uid="{D85F07D2-8350-4ED7-8B33-F7CA31166E0B}"/>
+    <hyperlink ref="M4" r:id="rId5" xr:uid="{F327B5B9-39C0-4E36-8260-EAE33FD2F23D}"/>
+    <hyperlink ref="N4" r:id="rId6" xr:uid="{2CD354E4-B66C-41FA-BDFD-8AFA1B4E8B5C}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{20339AF2-C8BA-4B30-AEE4-496788AD1DEB}"/>
+    <hyperlink ref="M5" r:id="rId8" xr:uid="{E7C43A6C-94BC-4043-9ECF-77B7D5DF1885}"/>
+    <hyperlink ref="D17" r:id="rId9" xr:uid="{3D16A510-B7FF-4D47-B98C-798854F2138A}"/>
+    <hyperlink ref="M6" r:id="rId10" xr:uid="{2E2C7FEC-FCC8-46D6-9F28-09008EFC2E98}"/>
+    <hyperlink ref="M8" r:id="rId11" xr:uid="{C1F46BD4-6CC0-40A9-81D2-1CE2EF3468B0}"/>
+    <hyperlink ref="M11" r:id="rId12" xr:uid="{36F051C4-93B2-4CA1-B88C-A4F7703E33AD}"/>
+    <hyperlink ref="M18" r:id="rId13" display="Admin@123" xr:uid="{9240E756-8D87-41B2-B88F-E7318A883255}"/>
+    <hyperlink ref="M20" r:id="rId14" xr:uid="{55D19047-56C1-49FE-9CCE-7D25FBDBF4B5}"/>
+    <hyperlink ref="M10" r:id="rId15" xr:uid="{15D24EA3-471F-4C1E-B4AD-34402BF33E77}"/>
+    <hyperlink ref="M17" r:id="rId16" xr:uid="{F3D351E3-E3DC-40A9-AD4B-8DD339B49D09}"/>
+    <hyperlink ref="M21" r:id="rId17" xr:uid="{A3AAD49F-A299-483D-B1A0-13A778A16041}"/>
+    <hyperlink ref="N5" r:id="rId18" xr:uid="{341F89AA-596A-4DA3-B806-A9BE76EDF4BC}"/>
+    <hyperlink ref="N6" r:id="rId19" xr:uid="{78CC411F-73E5-4722-9EA0-34121AB42845}"/>
+    <hyperlink ref="N8" r:id="rId20" xr:uid="{4CAC76BA-32D2-45A8-A5D7-EDDC3F152EA9}"/>
+    <hyperlink ref="N11" r:id="rId21" xr:uid="{4388A44E-59AD-4708-91C4-530E760F78F4}"/>
+    <hyperlink ref="N10" r:id="rId22" xr:uid="{D407EAC0-1091-4612-80FF-8D4FD29BB2D2}"/>
+    <hyperlink ref="N17" r:id="rId23" xr:uid="{16FB91A2-A1DC-4B32-8025-C328CD33494E}"/>
+    <hyperlink ref="N21" r:id="rId24" xr:uid="{03F9F991-6E42-41D0-8F37-6CEBCAF682CD}"/>
+    <hyperlink ref="N18" r:id="rId25" display="Admin@123" xr:uid="{A8129A54-3091-4463-8093-D69A20642FE6}"/>
+    <hyperlink ref="N19" r:id="rId26" xr:uid="{4FE7D3D7-5789-409A-A37D-9B6A7CE36AA3}"/>
+    <hyperlink ref="M7" r:id="rId27" xr:uid="{F7E0475C-BECA-44D4-8598-5466FA3F3C8D}"/>
+    <hyperlink ref="N7" r:id="rId28" xr:uid="{4996C6EC-8A3D-4BF8-9255-D8976D660284}"/>
+    <hyperlink ref="M9" r:id="rId29" xr:uid="{EC37FB4E-FD41-4BD4-888B-17599E0851E0}"/>
+    <hyperlink ref="N9" r:id="rId30" xr:uid="{3C2971C2-1D9C-4A98-81CD-06619C3FF246}"/>
+    <hyperlink ref="D14" r:id="rId31" xr:uid="{B6C0F823-494E-4294-96D5-9FCAA5223E6F}"/>
+    <hyperlink ref="M12" r:id="rId32" xr:uid="{C65FFAFE-4C1A-490A-BC23-344C6FD61C43}"/>
+    <hyperlink ref="M13" r:id="rId33" xr:uid="{59B714BA-CE77-461F-9CF7-47EC25791E08}"/>
+    <hyperlink ref="M14" r:id="rId34" xr:uid="{749C29F6-07B2-4B1A-AC57-43EB9FB7B60E}"/>
+    <hyperlink ref="N12" r:id="rId35" xr:uid="{9953B0C0-235B-4726-8007-8AD465206505}"/>
+    <hyperlink ref="N13" r:id="rId36" xr:uid="{5B268448-BA40-493C-999B-4CDB7D75DBFC}"/>
+    <hyperlink ref="N14" r:id="rId37" xr:uid="{4BC6D98A-2D01-49A2-A12E-E7ED1E6887F6}"/>
+    <hyperlink ref="D16" r:id="rId38" xr:uid="{8BB4EB86-E4AC-40F7-BB9F-2C54C3A33A80}"/>
+    <hyperlink ref="M16" r:id="rId39" xr:uid="{7246A40C-6325-4CA5-A6C9-5DF1854D7C01}"/>
+    <hyperlink ref="N16" r:id="rId40" xr:uid="{D2F84660-768E-49AA-992D-86B2C8CC7CFB}"/>
+    <hyperlink ref="D6" r:id="rId41" xr:uid="{210486E1-181F-434B-A7F4-6A41E5AC3574}"/>
+    <hyperlink ref="D7" r:id="rId42" xr:uid="{1BECB6E8-0DC5-415D-BE0C-CCF4117C771E}"/>
+    <hyperlink ref="D8" r:id="rId43" xr:uid="{01B86751-44DB-4618-85FF-6BCC7D7ACD15}"/>
+    <hyperlink ref="D9" r:id="rId44" xr:uid="{3CC30BD7-6508-4736-B850-C6D3D15D2886}"/>
+    <hyperlink ref="D10" r:id="rId45" xr:uid="{7B0BB163-86E7-42BD-95D0-25F8D6096A16}"/>
+    <hyperlink ref="D12" r:id="rId46" xr:uid="{5CE96045-BB7F-4DE8-ABC5-D7D8952C7AFF}"/>
+    <hyperlink ref="D18" r:id="rId47" xr:uid="{6D2C8D27-968F-43C4-B39C-EB203BB56A43}"/>
+    <hyperlink ref="D19" r:id="rId48" xr:uid="{D14DE1A8-04B4-4A11-A105-A04F3AA08FB4}"/>
+    <hyperlink ref="D20" r:id="rId49" xr:uid="{8601F8BB-0610-4FEB-BF33-2515FEA0C8C9}"/>
+    <hyperlink ref="D21" r:id="rId50" xr:uid="{46AFB659-8E60-4290-B464-A85F725F775A}"/>
+    <hyperlink ref="S3" r:id="rId51" xr:uid="{F5444E3D-813D-454F-96AC-BAE1AA6945CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC75FA6E-738B-4B34-8B51-3655C2EAED1B}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.90625" customWidth="1"/>
+    <col min="2" max="2" width="38.54296875" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="10" max="10" width="22.6328125" customWidth="1"/>
+    <col min="11" max="11" width="18.90625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="21" max="21" width="23.5546875" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" customWidth="1"/>
-    <col min="24" max="24" width="31.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" customWidth="1"/>
-    <col min="26" max="26" width="28.44140625" customWidth="1"/>
+    <col min="19" max="19" width="22.36328125" customWidth="1"/>
+    <col min="21" max="21" width="23.54296875" customWidth="1"/>
+    <col min="22" max="22" width="23.36328125" customWidth="1"/>
+    <col min="24" max="24" width="31.54296875" customWidth="1"/>
+    <col min="25" max="25" width="19.6328125" customWidth="1"/>
+    <col min="26" max="26" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3052,7 +4107,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>516</v>
       </c>
@@ -3117,7 +4172,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -3176,7 +4231,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>526</v>
       </c>
@@ -3220,7 +4275,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>526</v>
       </c>
@@ -3267,7 +4322,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>526</v>
       </c>
@@ -3314,7 +4369,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>526</v>
       </c>
@@ -3361,7 +4416,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>526</v>
       </c>
@@ -3408,7 +4463,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>526</v>
       </c>
@@ -3455,7 +4510,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>526</v>
       </c>
@@ -3502,7 +4557,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>526</v>
       </c>
@@ -3549,7 +4604,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>526</v>
       </c>
@@ -3596,7 +4651,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>540</v>
       </c>
@@ -3640,7 +4695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>540</v>
       </c>
@@ -3681,7 +4736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>540</v>
       </c>
@@ -3722,7 +4777,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>540</v>
       </c>
@@ -3763,7 +4818,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>540</v>
       </c>
@@ -3868,6 +4923,378 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7446F1-455D-4825-A6ED-84437499AA4D}">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="25.90625" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" customWidth="1"/>
+    <col min="14" max="14" width="25.6328125" customWidth="1"/>
+    <col min="16" max="16" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="B2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>565</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="P2" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>565</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B4" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>565</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="N4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B5" t="s">
+        <v>573</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>565</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="15" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>565</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="15" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B7" t="s">
+        <v>575</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>565</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="15" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E6820CE7-80BC-4ED6-AF23-A523CA29787B}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{CA98E24C-B31A-4F38-8A22-238381507FDA}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{5FA89D8C-7540-4B1F-A1A9-06330ADB5B38}"/>
+    <hyperlink ref="L2" r:id="rId4" xr:uid="{30EAB0A8-8493-418B-BE3E-E2DAFB49DE8E}"/>
+    <hyperlink ref="M2" r:id="rId5" xr:uid="{3055E40E-F8B0-4B56-9F4C-CA062217525B}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{F269EE1A-F088-4FB0-818A-0D9E172535A6}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{A2409E6E-00C2-4593-B2C0-0B513D5DB795}"/>
+    <hyperlink ref="K3" r:id="rId8" xr:uid="{F53FB584-0F6F-4651-B9D4-28F3EE52312F}"/>
+    <hyperlink ref="L3" r:id="rId9" xr:uid="{92060F21-3AB6-408F-A4BE-9D570259118F}"/>
+    <hyperlink ref="M3" r:id="rId10" xr:uid="{B1D18432-4351-4756-B837-20D5D5233AAF}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{69119AF9-4967-4BB0-BB34-DEA50AB59824}"/>
+    <hyperlink ref="E4" r:id="rId12" xr:uid="{89FB5844-25C1-45A6-8C7C-5D3B4C0FE578}"/>
+    <hyperlink ref="K4" r:id="rId13" xr:uid="{35D64277-D74E-4593-B784-5CC6D5EF770B}"/>
+    <hyperlink ref="L4" r:id="rId14" xr:uid="{40A700A4-D149-4827-8032-BD2A5FB71BAA}"/>
+    <hyperlink ref="M4" r:id="rId15" xr:uid="{F4712EFA-82AF-477A-A30F-519CC5C28319}"/>
+    <hyperlink ref="D5" r:id="rId16" xr:uid="{FAAA4A07-5C06-48C7-A860-0A8A0D7DB8FB}"/>
+    <hyperlink ref="E5" r:id="rId17" xr:uid="{C3B36261-987D-4B70-80E1-CA7E9D9A8020}"/>
+    <hyperlink ref="K5" r:id="rId18" xr:uid="{01628038-7C8B-4935-8A9B-B84A19EE3289}"/>
+    <hyperlink ref="L5" r:id="rId19" xr:uid="{B5831364-1090-4D23-9349-16612D826488}"/>
+    <hyperlink ref="D6" r:id="rId20" xr:uid="{B70468B0-C878-4DBF-B7B0-9472F5A4A05F}"/>
+    <hyperlink ref="E6" r:id="rId21" xr:uid="{7BB14FCD-F359-4E35-B134-739DD00EFCE8}"/>
+    <hyperlink ref="K6" r:id="rId22" xr:uid="{FB4F2ABB-5EBE-4A61-94AA-986F315E0AF7}"/>
+    <hyperlink ref="D7" r:id="rId23" xr:uid="{9DF70183-B7CC-4B8B-AAF2-A657F01BCBAC}"/>
+    <hyperlink ref="E7" r:id="rId24" xr:uid="{79EE269B-3EBB-4752-87BC-6D50D0C33DF7}"/>
+    <hyperlink ref="K7" r:id="rId25" xr:uid="{6C490373-5DD4-4125-89AD-257ECBF7A94B}"/>
+    <hyperlink ref="L7" r:id="rId26" xr:uid="{6B970CA1-9335-4458-AB73-D5EDA71BF81C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D06DFA-D6F9-4A05-B463-4DDA52F0E3E7}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
@@ -3875,18 +5302,18 @@
       <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +5393,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -4034,7 +5461,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -4102,7 +5529,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -4170,7 +5597,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -4238,7 +5665,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -4306,7 +5733,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -4371,7 +5798,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -4436,7 +5863,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -4501,7 +5928,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -4566,7 +5993,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -4631,7 +6058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4696,7 +6123,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -4761,7 +6188,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -4826,7 +6253,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -5310,7 +6737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7342C061-16F1-49A5-BA07-4D17E62E882D}">
   <dimension ref="A1:AM42"/>
   <sheetViews>
@@ -5318,30 +6745,30 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="42.109375" customWidth="1"/>
-    <col min="7" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="19.88671875" customWidth="1"/>
-    <col min="15" max="15" width="30.109375" customWidth="1"/>
-    <col min="16" max="21" width="28.44140625" customWidth="1"/>
-    <col min="22" max="23" width="22.109375" customWidth="1"/>
-    <col min="24" max="29" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="35.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.08984375" customWidth="1"/>
+    <col min="7" max="8" width="16.36328125" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
+    <col min="10" max="10" width="19.90625" customWidth="1"/>
+    <col min="11" max="11" width="19.90625" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="19.90625" customWidth="1"/>
+    <col min="15" max="15" width="30.08984375" customWidth="1"/>
+    <col min="16" max="21" width="28.453125" customWidth="1"/>
+    <col min="22" max="23" width="22.08984375" customWidth="1"/>
+    <col min="24" max="29" width="19.90625" customWidth="1"/>
     <col min="30" max="30" width="50" customWidth="1"/>
-    <col min="31" max="31" width="22.44140625" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" customWidth="1"/>
     <col min="35" max="35" width="22" customWidth="1"/>
-    <col min="36" max="36" width="21.44140625" customWidth="1"/>
+    <col min="36" max="36" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5454,7 +6881,7 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
     </row>
-    <row r="2" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -5483,7 +6910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -5530,7 +6957,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -5559,7 +6986,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -5588,7 +7015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -5617,7 +7044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -5646,7 +7073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>236</v>
       </c>
@@ -5676,7 +7103,7 @@
       </c>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:39" ht="67.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:39" ht="43.5" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>238</v>
       </c>
@@ -5732,7 +7159,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="67.8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:39" ht="43.5" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>248</v>
       </c>
@@ -5789,7 +7216,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="67.8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:39" ht="57.5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>250</v>
       </c>
@@ -5846,7 +7273,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="94.2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:39" ht="89.5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -5909,7 +7336,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="57" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:39" ht="57.5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -5966,7 +7393,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="67.8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:39" ht="39.5" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>260</v>
       </c>
@@ -6026,7 +7453,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="94.2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:39" ht="89.5" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>263</v>
       </c>
@@ -6089,7 +7516,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>266</v>
       </c>
@@ -6125,7 +7552,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>269</v>
       </c>
@@ -6191,7 +7618,7 @@
       </c>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>274</v>
       </c>
@@ -6221,7 +7648,7 @@
       </c>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>276</v>
       </c>
@@ -6274,7 +7701,7 @@
       <c r="Z20" s="15"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -6308,7 +7735,7 @@
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
     </row>
-    <row r="22" spans="1:34" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>280</v>
       </c>
@@ -6358,7 +7785,7 @@
       <c r="AD22" s="15"/>
       <c r="AH22" s="15"/>
     </row>
-    <row r="23" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>280</v>
       </c>
@@ -6405,7 +7832,7 @@
       <c r="AD23" s="15"/>
       <c r="AH23" s="15"/>
     </row>
-    <row r="24" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>284</v>
       </c>
@@ -6457,7 +7884,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>287</v>
       </c>
@@ -6501,7 +7928,7 @@
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
     </row>
-    <row r="26" spans="1:34" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>291</v>
       </c>
@@ -6554,7 +7981,7 @@
       <c r="Z26" s="15"/>
       <c r="AD26" s="23"/>
     </row>
-    <row r="27" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>294</v>
       </c>
@@ -6613,7 +8040,7 @@
       </c>
       <c r="AD27" s="23"/>
     </row>
-    <row r="28" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>294</v>
       </c>
@@ -6667,7 +8094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>294</v>
       </c>
@@ -6721,7 +8148,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>296</v>
       </c>
@@ -6772,7 +8199,7 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
     </row>
-    <row r="31" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>298</v>
       </c>
@@ -6823,7 +8250,7 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:34" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>300</v>
       </c>
@@ -6869,7 +8296,7 @@
       <c r="Y32" s="23"/>
       <c r="Z32" s="23"/>
     </row>
-    <row r="33" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>303</v>
       </c>
@@ -6922,7 +8349,7 @@
       <c r="Y33" s="23"/>
       <c r="Z33" s="23"/>
     </row>
-    <row r="34" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>306</v>
       </c>
@@ -6957,7 +8384,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>310</v>
       </c>
@@ -6989,7 +8416,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>313</v>
       </c>
@@ -7024,7 +8451,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>316</v>
       </c>
@@ -7056,7 +8483,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="50" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>318</v>
       </c>
@@ -7141,7 +8568,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -7184,7 +8611,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>332</v>
       </c>
@@ -7219,7 +8646,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>333</v>
       </c>
@@ -7344,7 +8771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F2C328-44FE-4BE7-9D79-D8AE6FF7329F}">
   <dimension ref="A1:S15"/>
   <sheetViews>
@@ -7352,28 +8779,28 @@
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="2" max="2" width="43.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="43.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
-    <col min="14" max="15" width="13.44140625" customWidth="1"/>
-    <col min="17" max="17" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="43.453125" customWidth="1"/>
+    <col min="5" max="5" width="21.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" customWidth="1"/>
+    <col min="9" max="9" width="15.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" customWidth="1"/>
+    <col min="11" max="11" width="19.90625" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" customWidth="1"/>
+    <col min="14" max="15" width="13.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.453125" customWidth="1"/>
     <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7897,7 +9324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD7EB4D-1B81-49AC-A852-CF79C3CF942B}">
   <dimension ref="A1:X18"/>
   <sheetViews>
@@ -7905,22 +9332,22 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.453125" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
-    <col min="23" max="23" width="9.44140625" customWidth="1"/>
+    <col min="23" max="23" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7994,7 +9421,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>335</v>
       </c>
@@ -8059,7 +9486,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>341</v>
       </c>
@@ -8127,7 +9554,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -8192,7 +9619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>352</v>
       </c>
@@ -8225,7 +9652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>353</v>
       </c>
@@ -8290,7 +9717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -8355,7 +9782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>353</v>
       </c>
@@ -8429,7 +9856,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>353</v>
       </c>
@@ -8497,7 +9924,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>353</v>
       </c>
@@ -8565,7 +9992,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>353</v>
       </c>
@@ -8633,7 +10060,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>353</v>
       </c>
@@ -8701,7 +10128,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>353</v>
       </c>
@@ -8770,7 +10197,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>353</v>
       </c>
@@ -8838,7 +10265,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>353</v>
       </c>
@@ -8906,7 +10333,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>353</v>
       </c>
@@ -8974,7 +10401,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -9042,7 +10469,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>353</v>
       </c>
@@ -9122,7 +10549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9132,14 +10559,14 @@
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9147,985 +10574,9 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B18C423-D7E7-4B7B-9167-D2BDC190AA4E}">
-  <dimension ref="A1:W22"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.44140625" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="5" max="5" width="35.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="49.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="18" width="19.33203125" customWidth="1"/>
-    <col min="19" max="19" width="22.6640625" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>397</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>400</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>443</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>445</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>446</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>447</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>448</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>449</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>454</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>405</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>456</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="20" t="s">
-        <v>457</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>463</v>
-      </c>
-      <c r="I4" t="s">
-        <v>442</v>
-      </c>
-      <c r="J4" t="s">
-        <v>442</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>464</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>464</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>466</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I5" s="19"/>
-      <c r="J5" t="s">
-        <v>456</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U5" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B6" t="s">
-        <v>470</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U6" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="20" t="s">
-        <v>474</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J7" t="s">
-        <v>456</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="V7" t="s">
-        <v>49</v>
-      </c>
-      <c r="W7" s="14" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B8" t="s">
-        <v>476</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="I8" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J8" t="s">
-        <v>456</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B9" t="s">
-        <v>477</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="20" t="s">
-        <v>478</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J9" t="s">
-        <v>456</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="V9" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="14" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B10" t="s">
-        <v>480</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>481</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J10" t="s">
-        <v>456</v>
-      </c>
-      <c r="K10" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P10" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B11" t="s">
-        <v>482</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" t="s">
-        <v>483</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J11" t="s">
-        <v>456</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U11" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B12" t="s">
-        <v>485</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J12" t="s">
-        <v>456</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U12" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B13" t="s">
-        <v>487</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J13" t="s">
-        <v>456</v>
-      </c>
-      <c r="K13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O13" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U13" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B14" t="s">
-        <v>489</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J14" t="s">
-        <v>456</v>
-      </c>
-      <c r="K14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="V14" t="s">
-        <v>49</v>
-      </c>
-      <c r="W14" s="14" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B15" t="s">
-        <v>491</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>492</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="F15" s="20"/>
-      <c r="I15" s="19"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U15" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B16" t="s">
-        <v>493</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J16" t="s">
-        <v>456</v>
-      </c>
-      <c r="K16" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U16" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J17" t="s">
-        <v>456</v>
-      </c>
-      <c r="K17" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O17" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="U17" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B18" t="s">
-        <v>496</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J18" t="s">
-        <v>456</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="O18" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B19" t="s">
-        <v>499</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>500</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J19" t="s">
-        <v>456</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B20" t="s">
-        <v>501</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J20" t="s">
-        <v>456</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B21" t="s">
-        <v>502</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J21" t="s">
-        <v>456</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="O21" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="B22" t="s">
-        <v>504</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>505</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{40B15EDC-AE23-443B-B49A-CCCCBA695541}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{34364467-99E6-4A73-9F0A-367BEB8795A2}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{76ED8F48-D6F5-4471-9E0F-F1693D3E4241}"/>
-    <hyperlink ref="D4" r:id="rId4" display="a@b.in,a@b.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghiklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com,a@bcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefgdhijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyzabcdefghijklmnopq.com" xr:uid="{D85F07D2-8350-4ED7-8B33-F7CA31166E0B}"/>
-    <hyperlink ref="M4" r:id="rId5" xr:uid="{F327B5B9-39C0-4E36-8260-EAE33FD2F23D}"/>
-    <hyperlink ref="N4" r:id="rId6" xr:uid="{2CD354E4-B66C-41FA-BDFD-8AFA1B4E8B5C}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{20339AF2-C8BA-4B30-AEE4-496788AD1DEB}"/>
-    <hyperlink ref="M5" r:id="rId8" xr:uid="{E7C43A6C-94BC-4043-9ECF-77B7D5DF1885}"/>
-    <hyperlink ref="D17" r:id="rId9" xr:uid="{3D16A510-B7FF-4D47-B98C-798854F2138A}"/>
-    <hyperlink ref="M6" r:id="rId10" xr:uid="{2E2C7FEC-FCC8-46D6-9F28-09008EFC2E98}"/>
-    <hyperlink ref="M8" r:id="rId11" xr:uid="{C1F46BD4-6CC0-40A9-81D2-1CE2EF3468B0}"/>
-    <hyperlink ref="M11" r:id="rId12" xr:uid="{36F051C4-93B2-4CA1-B88C-A4F7703E33AD}"/>
-    <hyperlink ref="M18" r:id="rId13" display="Admin@123" xr:uid="{9240E756-8D87-41B2-B88F-E7318A883255}"/>
-    <hyperlink ref="M20" r:id="rId14" xr:uid="{55D19047-56C1-49FE-9CCE-7D25FBDBF4B5}"/>
-    <hyperlink ref="M10" r:id="rId15" xr:uid="{15D24EA3-471F-4C1E-B4AD-34402BF33E77}"/>
-    <hyperlink ref="M17" r:id="rId16" xr:uid="{F3D351E3-E3DC-40A9-AD4B-8DD339B49D09}"/>
-    <hyperlink ref="M21" r:id="rId17" xr:uid="{A3AAD49F-A299-483D-B1A0-13A778A16041}"/>
-    <hyperlink ref="N5" r:id="rId18" xr:uid="{341F89AA-596A-4DA3-B806-A9BE76EDF4BC}"/>
-    <hyperlink ref="N6" r:id="rId19" xr:uid="{78CC411F-73E5-4722-9EA0-34121AB42845}"/>
-    <hyperlink ref="N8" r:id="rId20" xr:uid="{4CAC76BA-32D2-45A8-A5D7-EDDC3F152EA9}"/>
-    <hyperlink ref="N11" r:id="rId21" xr:uid="{4388A44E-59AD-4708-91C4-530E760F78F4}"/>
-    <hyperlink ref="N10" r:id="rId22" xr:uid="{D407EAC0-1091-4612-80FF-8D4FD29BB2D2}"/>
-    <hyperlink ref="N17" r:id="rId23" xr:uid="{16FB91A2-A1DC-4B32-8025-C328CD33494E}"/>
-    <hyperlink ref="N21" r:id="rId24" xr:uid="{03F9F991-6E42-41D0-8F37-6CEBCAF682CD}"/>
-    <hyperlink ref="N18" r:id="rId25" display="Admin@123" xr:uid="{A8129A54-3091-4463-8093-D69A20642FE6}"/>
-    <hyperlink ref="N19" r:id="rId26" xr:uid="{4FE7D3D7-5789-409A-A37D-9B6A7CE36AA3}"/>
-    <hyperlink ref="M7" r:id="rId27" xr:uid="{F7E0475C-BECA-44D4-8598-5466FA3F3C8D}"/>
-    <hyperlink ref="N7" r:id="rId28" xr:uid="{4996C6EC-8A3D-4BF8-9255-D8976D660284}"/>
-    <hyperlink ref="M9" r:id="rId29" xr:uid="{EC37FB4E-FD41-4BD4-888B-17599E0851E0}"/>
-    <hyperlink ref="N9" r:id="rId30" xr:uid="{3C2971C2-1D9C-4A98-81CD-06619C3FF246}"/>
-    <hyperlink ref="D14" r:id="rId31" xr:uid="{B6C0F823-494E-4294-96D5-9FCAA5223E6F}"/>
-    <hyperlink ref="M12" r:id="rId32" xr:uid="{C65FFAFE-4C1A-490A-BC23-344C6FD61C43}"/>
-    <hyperlink ref="M13" r:id="rId33" xr:uid="{59B714BA-CE77-461F-9CF7-47EC25791E08}"/>
-    <hyperlink ref="M14" r:id="rId34" xr:uid="{749C29F6-07B2-4B1A-AC57-43EB9FB7B60E}"/>
-    <hyperlink ref="N12" r:id="rId35" xr:uid="{9953B0C0-235B-4726-8007-8AD465206505}"/>
-    <hyperlink ref="N13" r:id="rId36" xr:uid="{5B268448-BA40-493C-999B-4CDB7D75DBFC}"/>
-    <hyperlink ref="N14" r:id="rId37" xr:uid="{4BC6D98A-2D01-49A2-A12E-E7ED1E6887F6}"/>
-    <hyperlink ref="D16" r:id="rId38" xr:uid="{8BB4EB86-E4AC-40F7-BB9F-2C54C3A33A80}"/>
-    <hyperlink ref="M16" r:id="rId39" xr:uid="{7246A40C-6325-4CA5-A6C9-5DF1854D7C01}"/>
-    <hyperlink ref="N16" r:id="rId40" xr:uid="{D2F84660-768E-49AA-992D-86B2C8CC7CFB}"/>
-    <hyperlink ref="D6" r:id="rId41" xr:uid="{210486E1-181F-434B-A7F4-6A41E5AC3574}"/>
-    <hyperlink ref="D7" r:id="rId42" xr:uid="{1BECB6E8-0DC5-415D-BE0C-CCF4117C771E}"/>
-    <hyperlink ref="D8" r:id="rId43" xr:uid="{01B86751-44DB-4618-85FF-6BCC7D7ACD15}"/>
-    <hyperlink ref="D9" r:id="rId44" xr:uid="{3CC30BD7-6508-4736-B850-C6D3D15D2886}"/>
-    <hyperlink ref="D10" r:id="rId45" xr:uid="{7B0BB163-86E7-42BD-95D0-25F8D6096A16}"/>
-    <hyperlink ref="D12" r:id="rId46" xr:uid="{5CE96045-BB7F-4DE8-ABC5-D7D8952C7AFF}"/>
-    <hyperlink ref="D18" r:id="rId47" xr:uid="{6D2C8D27-968F-43C4-B39C-EB203BB56A43}"/>
-    <hyperlink ref="D19" r:id="rId48" xr:uid="{D14DE1A8-04B4-4A11-A105-A04F3AA08FB4}"/>
-    <hyperlink ref="D20" r:id="rId49" xr:uid="{8601F8BB-0610-4FEB-BF33-2515FEA0C8C9}"/>
-    <hyperlink ref="D21" r:id="rId50" xr:uid="{46AFB659-8E60-4290-B464-A85F725F775A}"/>
-    <hyperlink ref="S3" r:id="rId51" xr:uid="{F5444E3D-813D-454F-96AC-BAE1AA6945CE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Written test Script for Token Account -Withdrawn Gift Card
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (17-01-2021)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (19-01-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328122F1-30D0-42C8-A15E-E1383AE882AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74165BC3-C49A-4097-A3AE-08DF61DFD803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="User-Details" sheetId="10" r:id="rId2"/>
     <sheet name="changePassword" sheetId="11" r:id="rId3"/>
-    <sheet name="PaymentMethods" sheetId="4" r:id="rId4"/>
-    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId5"/>
-    <sheet name="forgotEmail" sheetId="6" r:id="rId6"/>
-    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId7"/>
-    <sheet name="filters" sheetId="3" r:id="rId8"/>
-    <sheet name="profile" sheetId="2" r:id="rId9"/>
-    <sheet name="homePage" sheetId="9" r:id="rId10"/>
+    <sheet name="withdrawnGiftCard" sheetId="12" r:id="rId4"/>
+    <sheet name="PaymentMethods" sheetId="4" r:id="rId5"/>
+    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId6"/>
+    <sheet name="forgotEmail" sheetId="6" r:id="rId7"/>
+    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId8"/>
+    <sheet name="filters" sheetId="3" r:id="rId9"/>
+    <sheet name="profile" sheetId="2" r:id="rId10"/>
+    <sheet name="homePage" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="613">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1779,6 +1780,111 @@
   </si>
   <si>
     <t>New password should not match with Old password</t>
+  </si>
+  <si>
+    <t>giftHeading</t>
+  </si>
+  <si>
+    <t>orderHeading</t>
+  </si>
+  <si>
+    <t>authyHeading1</t>
+  </si>
+  <si>
+    <t>successHeading</t>
+  </si>
+  <si>
+    <t>searchKey</t>
+  </si>
+  <si>
+    <t>searchKey1</t>
+  </si>
+  <si>
+    <t>test gift card with Amazon</t>
+  </si>
+  <si>
+    <t>giftcard-Amazon</t>
+  </si>
+  <si>
+    <t>Gift Card Purchase</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Order Preview</t>
+  </si>
+  <si>
+    <t>Transaction in Progress</t>
+  </si>
+  <si>
+    <t>Am</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>test gift card with Visa</t>
+  </si>
+  <si>
+    <t>giftcard-Visa</t>
+  </si>
+  <si>
+    <t>test gift card navigation</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>test gift card amazon  with invalid data</t>
+  </si>
+  <si>
+    <t>Empty First Name</t>
+  </si>
+  <si>
+    <t>First Name is required</t>
+  </si>
+  <si>
+    <t>Special Character</t>
+  </si>
+  <si>
+    <t>#@</t>
+  </si>
+  <si>
+    <t>Only alphabets are allowed</t>
+  </si>
+  <si>
+    <t>Empty Last Name</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Last Name is required</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Empty Amount</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Amount must be more than or equal to $0.01 USD</t>
+  </si>
+  <si>
+    <t>a@b.in</t>
+  </si>
+  <si>
+    <t>as@v</t>
+  </si>
+  <si>
+    <t>test gift card visa  with invalid data</t>
+  </si>
+  <si>
+    <t>Amount must be more than or equal to $5.00 USD</t>
   </si>
 </sst>
 </file>
@@ -1828,6 +1934,7 @@
       <sz val="8"/>
       <color rgb="FF242424"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2368,25 +2475,25 @@
       <selection pane="topRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.453125" customWidth="1"/>
-    <col min="2" max="2" width="50.08984375" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
-    <col min="6" max="6" width="63.90625" customWidth="1"/>
-    <col min="7" max="7" width="63.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="63.88671875" customWidth="1"/>
+    <col min="7" max="7" width="63.44140625" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43" customWidth="1"/>
-    <col min="10" max="10" width="33.90625" customWidth="1"/>
-    <col min="11" max="11" width="24.453125" customWidth="1"/>
-    <col min="12" max="12" width="26.453125" customWidth="1"/>
-    <col min="13" max="13" width="32.90625" customWidth="1"/>
-    <col min="14" max="14" width="22.90625" customWidth="1"/>
+    <col min="10" max="10" width="33.88671875" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.44140625" customWidth="1"/>
+    <col min="13" max="13" width="32.88671875" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2451,7 +2558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2480,7 +2587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2510,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2540,7 +2647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2569,7 +2676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2601,7 +2708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2630,7 +2737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2648,7 +2755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2686,7 +2793,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2718,7 +2825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2750,7 +2857,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2782,7 +2889,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2814,7 +2921,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2837,7 +2944,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2869,7 +2976,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -2898,7 +3005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2924,7 +3031,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2950,7 +3057,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2976,7 +3083,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -3019,6 +3126,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B18C423-D7E7-4B7B-9167-D2BDC190AA4E}">
   <dimension ref="A1:W22"/>
   <sheetViews>
@@ -3026,29 +3148,29 @@
       <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.453125" customWidth="1"/>
-    <col min="2" max="2" width="48.36328125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" customWidth="1"/>
-    <col min="5" max="5" width="35.90625" customWidth="1"/>
-    <col min="6" max="6" width="35.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
-    <col min="9" max="9" width="49.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" customWidth="1"/>
-    <col min="15" max="15" width="19.36328125" customWidth="1"/>
-    <col min="16" max="16" width="23.6328125" customWidth="1"/>
-    <col min="17" max="18" width="19.36328125" customWidth="1"/>
-    <col min="19" max="19" width="22.6328125" customWidth="1"/>
-    <col min="20" max="20" width="19.36328125" customWidth="1"/>
+    <col min="1" max="1" width="49.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="49.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" customWidth="1"/>
+    <col min="17" max="18" width="19.33203125" customWidth="1"/>
+    <col min="19" max="19" width="22.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3119,7 +3241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>449</v>
       </c>
@@ -3151,7 +3273,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" spans="1:23" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>452</v>
       </c>
@@ -4002,32 +4124,32 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.90625" customWidth="1"/>
-    <col min="2" max="2" width="38.54296875" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="28.54296875" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" customWidth="1"/>
-    <col min="10" max="10" width="22.6328125" customWidth="1"/>
-    <col min="11" max="11" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="22.36328125" customWidth="1"/>
-    <col min="21" max="21" width="23.54296875" customWidth="1"/>
-    <col min="22" max="22" width="23.36328125" customWidth="1"/>
-    <col min="24" max="24" width="31.54296875" customWidth="1"/>
-    <col min="25" max="25" width="19.6328125" customWidth="1"/>
-    <col min="26" max="26" width="28.453125" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="21" max="21" width="23.5546875" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" customWidth="1"/>
+    <col min="24" max="24" width="31.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" customWidth="1"/>
+    <col min="26" max="26" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4107,7 +4229,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>516</v>
       </c>
@@ -4172,7 +4294,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -4231,7 +4353,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>526</v>
       </c>
@@ -4275,7 +4397,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>526</v>
       </c>
@@ -4322,7 +4444,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>526</v>
       </c>
@@ -4369,7 +4491,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>526</v>
       </c>
@@ -4416,7 +4538,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>526</v>
       </c>
@@ -4463,7 +4585,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>526</v>
       </c>
@@ -4510,7 +4632,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>526</v>
       </c>
@@ -4557,7 +4679,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>526</v>
       </c>
@@ -4604,7 +4726,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>526</v>
       </c>
@@ -4651,7 +4773,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>540</v>
       </c>
@@ -4695,7 +4817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>540</v>
       </c>
@@ -4736,7 +4858,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>540</v>
       </c>
@@ -4777,7 +4899,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>540</v>
       </c>
@@ -4818,7 +4940,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>540</v>
       </c>
@@ -4926,30 +5048,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7446F1-455D-4825-A6ED-84437499AA4D}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.54296875" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" customWidth="1"/>
-    <col min="9" max="9" width="25.90625" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" customWidth="1"/>
-    <col min="12" max="12" width="13.6328125" customWidth="1"/>
-    <col min="13" max="13" width="17.1796875" customWidth="1"/>
-    <col min="14" max="14" width="25.6328125" customWidth="1"/>
-    <col min="16" max="16" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5002,7 +5124,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="64.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>561</v>
       </c>
@@ -5052,7 +5174,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>561</v>
       </c>
@@ -5093,7 +5215,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>568</v>
       </c>
@@ -5137,7 +5259,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>568</v>
       </c>
@@ -5179,7 +5301,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>568</v>
       </c>
@@ -5219,7 +5341,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>568</v>
       </c>
@@ -5295,6 +5417,843 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0341D91D-2664-4CF3-AF4B-EBD6A1B18156}">
+  <dimension ref="A1:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" customWidth="1"/>
+    <col min="19" max="19" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F2" t="s">
+        <v>564</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>586</v>
+      </c>
+      <c r="K2" t="s">
+        <v>455</v>
+      </c>
+      <c r="L2" t="s">
+        <v>587</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>588</v>
+      </c>
+      <c r="O2" t="s">
+        <v>226</v>
+      </c>
+      <c r="P2" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>590</v>
+      </c>
+      <c r="R2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F3" t="s">
+        <v>564</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>586</v>
+      </c>
+      <c r="K3" t="s">
+        <v>455</v>
+      </c>
+      <c r="L3" t="s">
+        <v>587</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" t="s">
+        <v>588</v>
+      </c>
+      <c r="O3" t="s">
+        <v>226</v>
+      </c>
+      <c r="P3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B4" t="s">
+        <v>595</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F4" t="s">
+        <v>564</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>586</v>
+      </c>
+      <c r="K4" t="s">
+        <v>455</v>
+      </c>
+      <c r="L4" t="s">
+        <v>587</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>588</v>
+      </c>
+      <c r="O4" t="s">
+        <v>226</v>
+      </c>
+      <c r="P4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>596</v>
+      </c>
+      <c r="B5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" t="s">
+        <v>564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>586</v>
+      </c>
+      <c r="S5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B6" t="s">
+        <v>599</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F6" t="s">
+        <v>564</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>586</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="S6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>596</v>
+      </c>
+      <c r="B7" t="s">
+        <v>602</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F7" t="s">
+        <v>564</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>586</v>
+      </c>
+      <c r="K7" t="s">
+        <v>603</v>
+      </c>
+      <c r="S7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>596</v>
+      </c>
+      <c r="B8" t="s">
+        <v>599</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" t="s">
+        <v>564</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>586</v>
+      </c>
+      <c r="K8" t="s">
+        <v>603</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="S8" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>596</v>
+      </c>
+      <c r="B9" t="s">
+        <v>482</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F9" t="s">
+        <v>564</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>586</v>
+      </c>
+      <c r="K9" t="s">
+        <v>603</v>
+      </c>
+      <c r="L9" t="s">
+        <v>605</v>
+      </c>
+      <c r="S9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>596</v>
+      </c>
+      <c r="B10" t="s">
+        <v>606</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F10" t="s">
+        <v>564</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>586</v>
+      </c>
+      <c r="K10" t="s">
+        <v>603</v>
+      </c>
+      <c r="L10" t="s">
+        <v>605</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="S10" t="s">
+        <v>608</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>596</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F11" t="s">
+        <v>564</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>586</v>
+      </c>
+      <c r="K11" t="s">
+        <v>603</v>
+      </c>
+      <c r="L11" t="s">
+        <v>605</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>611</v>
+      </c>
+      <c r="B12" t="s">
+        <v>597</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F12" t="s">
+        <v>564</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>586</v>
+      </c>
+      <c r="S12" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>611</v>
+      </c>
+      <c r="B13" t="s">
+        <v>599</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F13" t="s">
+        <v>564</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s">
+        <v>586</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="S13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>611</v>
+      </c>
+      <c r="B14" t="s">
+        <v>602</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F14" t="s">
+        <v>564</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" t="s">
+        <v>586</v>
+      </c>
+      <c r="K14" t="s">
+        <v>603</v>
+      </c>
+      <c r="S14" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>611</v>
+      </c>
+      <c r="B15" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F15" t="s">
+        <v>564</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>586</v>
+      </c>
+      <c r="K15" t="s">
+        <v>603</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="S15" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>611</v>
+      </c>
+      <c r="B16" t="s">
+        <v>482</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F16" t="s">
+        <v>564</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>586</v>
+      </c>
+      <c r="K16" t="s">
+        <v>603</v>
+      </c>
+      <c r="L16" t="s">
+        <v>605</v>
+      </c>
+      <c r="S16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>611</v>
+      </c>
+      <c r="B17" t="s">
+        <v>606</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F17" t="s">
+        <v>564</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" t="s">
+        <v>586</v>
+      </c>
+      <c r="K17" t="s">
+        <v>603</v>
+      </c>
+      <c r="L17" t="s">
+        <v>605</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="S17" t="s">
+        <v>612</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F18" t="s">
+        <v>564</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="s">
+        <v>586</v>
+      </c>
+      <c r="K18" t="s">
+        <v>603</v>
+      </c>
+      <c r="L18" t="s">
+        <v>605</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" t="s">
+        <v>43</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T10" r:id="rId1" xr:uid="{C2AFA401-054D-46CB-B95A-1346B643AB6F}"/>
+    <hyperlink ref="T11" r:id="rId2" xr:uid="{2FC5DD4A-AABB-473E-84AD-1DEE99166B94}"/>
+    <hyperlink ref="K6" r:id="rId3" xr:uid="{15488999-BE22-4B4A-B568-679FD5AD013A}"/>
+    <hyperlink ref="T17" r:id="rId4" xr:uid="{66B8B0A3-C9A9-4133-9FE0-C91F8DD11583}"/>
+    <hyperlink ref="T18" r:id="rId5" xr:uid="{04EDCA02-3714-4786-905A-6CB3F98AAE0A}"/>
+    <hyperlink ref="K13" r:id="rId6" xr:uid="{328D2DC3-5A78-4770-9E93-1A0176B33F12}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{078068CE-1034-4759-A12F-A2A2838F8004}"/>
+    <hyperlink ref="L15" r:id="rId8" xr:uid="{673C5022-29E0-4E2E-BD78-1CFF0F626F8E}"/>
+    <hyperlink ref="D2" r:id="rId9" xr:uid="{CC366F0B-F833-4745-98C4-EDFF1420101F}"/>
+    <hyperlink ref="D3:D18" r:id="rId10" display="maniv789396@gmail.com" xr:uid="{940DD7FE-36D1-40F6-B667-25B63DAEEF12}"/>
+    <hyperlink ref="E2" r:id="rId11" xr:uid="{7183412E-3337-439A-B15A-9549BCD7A19F}"/>
+    <hyperlink ref="E3:E18" r:id="rId12" display="Admin@123" xr:uid="{C4B12101-0794-4314-893F-FC20EF83F793}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D06DFA-D6F9-4A05-B463-4DDA52F0E3E7}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
@@ -5302,18 +6261,18 @@
       <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5393,7 +6352,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -5461,7 +6420,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -5529,7 +6488,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -5597,7 +6556,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -5665,7 +6624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -5733,7 +6692,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -5798,7 +6757,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -5863,7 +6822,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -5928,7 +6887,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -5993,7 +6952,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -6058,7 +7017,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -6123,7 +7082,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -6188,7 +7147,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -6253,7 +7212,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -6737,7 +7696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7342C061-16F1-49A5-BA07-4D17E62E882D}">
   <dimension ref="A1:AM42"/>
   <sheetViews>
@@ -6745,30 +7704,30 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="35.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="42.08984375" customWidth="1"/>
-    <col min="7" max="8" width="16.36328125" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="19.90625" customWidth="1"/>
-    <col min="11" max="11" width="19.90625" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="19.90625" customWidth="1"/>
-    <col min="15" max="15" width="30.08984375" customWidth="1"/>
-    <col min="16" max="21" width="28.453125" customWidth="1"/>
-    <col min="22" max="23" width="22.08984375" customWidth="1"/>
-    <col min="24" max="29" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" customWidth="1"/>
+    <col min="7" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="19.88671875" customWidth="1"/>
+    <col min="15" max="15" width="30.109375" customWidth="1"/>
+    <col min="16" max="21" width="28.44140625" customWidth="1"/>
+    <col min="22" max="23" width="22.109375" customWidth="1"/>
+    <col min="24" max="29" width="19.88671875" customWidth="1"/>
     <col min="30" max="30" width="50" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" customWidth="1"/>
+    <col min="31" max="31" width="22.44140625" customWidth="1"/>
     <col min="35" max="35" width="22" customWidth="1"/>
-    <col min="36" max="36" width="21.453125" customWidth="1"/>
+    <col min="36" max="36" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6881,7 +7840,7 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
     </row>
-    <row r="2" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -6910,7 +7869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -6957,7 +7916,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -6986,7 +7945,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -7015,7 +7974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -7044,7 +8003,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -7073,7 +8032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>236</v>
       </c>
@@ -7103,7 +8062,7 @@
       </c>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:39" ht="43.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:39" ht="43.2" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
         <v>238</v>
       </c>
@@ -7159,7 +8118,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="43.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" ht="43.2" x14ac:dyDescent="0.4">
       <c r="A10" s="15" t="s">
         <v>248</v>
       </c>
@@ -7216,7 +8175,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="57.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" ht="57" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>250</v>
       </c>
@@ -7273,7 +8232,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="89.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:39" ht="94.2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -7336,7 +8295,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="57.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:39" ht="57" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -7393,7 +8352,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="39.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:39" ht="41.4" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
         <v>260</v>
       </c>
@@ -7453,7 +8412,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="89.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" ht="94.2" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>263</v>
       </c>
@@ -7516,7 +8475,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>266</v>
       </c>
@@ -7552,7 +8511,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>269</v>
       </c>
@@ -7618,7 +8577,7 @@
       </c>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>274</v>
       </c>
@@ -7648,7 +8607,7 @@
       </c>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>276</v>
       </c>
@@ -7701,7 +8660,7 @@
       <c r="Z20" s="15"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -7735,7 +8694,7 @@
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
     </row>
-    <row r="22" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>280</v>
       </c>
@@ -7785,7 +8744,7 @@
       <c r="AD22" s="15"/>
       <c r="AH22" s="15"/>
     </row>
-    <row r="23" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>280</v>
       </c>
@@ -7832,7 +8791,7 @@
       <c r="AD23" s="15"/>
       <c r="AH23" s="15"/>
     </row>
-    <row r="24" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>284</v>
       </c>
@@ -7884,7 +8843,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>287</v>
       </c>
@@ -7928,7 +8887,7 @@
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
     </row>
-    <row r="26" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>291</v>
       </c>
@@ -7981,7 +8940,7 @@
       <c r="Z26" s="15"/>
       <c r="AD26" s="23"/>
     </row>
-    <row r="27" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>294</v>
       </c>
@@ -8040,7 +8999,7 @@
       </c>
       <c r="AD27" s="23"/>
     </row>
-    <row r="28" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>294</v>
       </c>
@@ -8094,7 +9053,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>294</v>
       </c>
@@ -8148,7 +9107,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>296</v>
       </c>
@@ -8199,7 +9158,7 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
     </row>
-    <row r="31" spans="1:34" ht="25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>298</v>
       </c>
@@ -8250,7 +9209,7 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:34" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>300</v>
       </c>
@@ -8296,7 +9255,7 @@
       <c r="Y32" s="23"/>
       <c r="Z32" s="23"/>
     </row>
-    <row r="33" spans="1:26" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>303</v>
       </c>
@@ -8349,7 +9308,7 @@
       <c r="Y33" s="23"/>
       <c r="Z33" s="23"/>
     </row>
-    <row r="34" spans="1:26" ht="50" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>306</v>
       </c>
@@ -8384,7 +9343,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>310</v>
       </c>
@@ -8416,7 +9375,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="50" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>313</v>
       </c>
@@ -8451,7 +9410,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>316</v>
       </c>
@@ -8483,7 +9442,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="50" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>318</v>
       </c>
@@ -8568,7 +9527,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -8611,7 +9570,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>332</v>
       </c>
@@ -8646,7 +9605,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>333</v>
       </c>
@@ -8771,7 +9730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F2C328-44FE-4BE7-9D79-D8AE6FF7329F}">
   <dimension ref="A1:S15"/>
   <sheetViews>
@@ -8779,28 +9738,28 @@
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" customWidth="1"/>
-    <col min="2" max="2" width="43.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="43.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.90625" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.08984375" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" customWidth="1"/>
-    <col min="11" max="11" width="19.90625" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" customWidth="1"/>
-    <col min="14" max="15" width="13.453125" customWidth="1"/>
-    <col min="17" max="17" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="43.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="14" max="15" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" customWidth="1"/>
     <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="16.54296875" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9324,7 +10283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD7EB4D-1B81-49AC-A852-CF79C3CF942B}">
   <dimension ref="A1:X18"/>
   <sheetViews>
@@ -9332,22 +10291,22 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
-    <col min="2" max="2" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.44140625" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
-    <col min="23" max="23" width="9.453125" customWidth="1"/>
+    <col min="23" max="23" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9421,7 +10380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>335</v>
       </c>
@@ -9486,7 +10445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>341</v>
       </c>
@@ -9554,7 +10513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -9619,7 +10578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>352</v>
       </c>
@@ -9652,7 +10611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>353</v>
       </c>
@@ -9717,7 +10676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -9782,7 +10741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>353</v>
       </c>
@@ -9856,7 +10815,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>353</v>
       </c>
@@ -9924,7 +10883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>353</v>
       </c>
@@ -9992,7 +10951,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>353</v>
       </c>
@@ -10060,7 +11019,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>353</v>
       </c>
@@ -10128,7 +11087,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>353</v>
       </c>
@@ -10197,7 +11156,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>353</v>
       </c>
@@ -10265,7 +11224,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>353</v>
       </c>
@@ -10333,7 +11292,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>353</v>
       </c>
@@ -10401,7 +11360,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -10469,7 +11428,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>353</v>
       </c>
@@ -10549,7 +11508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10559,22 +11518,7 @@
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Token Account-WithdrawntoUSD - External Bank Account
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata.xlsx
+++ b/Web/coyni/resources/testdata.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (19-01-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web (24-01-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74165BC3-C49A-4097-A3AE-08DF61DFD803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3695BA-963C-403F-8B0E-1C8992C6445F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="User-Details" sheetId="10" r:id="rId2"/>
     <sheet name="changePassword" sheetId="11" r:id="rId3"/>
     <sheet name="withdrawnGiftCard" sheetId="12" r:id="rId4"/>
-    <sheet name="PaymentMethods" sheetId="4" r:id="rId5"/>
-    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId6"/>
-    <sheet name="forgotEmail" sheetId="6" r:id="rId7"/>
-    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId8"/>
-    <sheet name="filters" sheetId="3" r:id="rId9"/>
-    <sheet name="profile" sheetId="2" r:id="rId10"/>
-    <sheet name="homePage" sheetId="9" r:id="rId11"/>
+    <sheet name="withdrawnToUSDExternalBank" sheetId="13" r:id="rId5"/>
+    <sheet name="PaymentMethods" sheetId="4" r:id="rId6"/>
+    <sheet name="TokenAccount-Customer" sheetId="5" r:id="rId7"/>
+    <sheet name="forgotEmail" sheetId="6" r:id="rId8"/>
+    <sheet name="PaymentMethods-Debit" sheetId="7" r:id="rId9"/>
+    <sheet name="filters" sheetId="3" r:id="rId10"/>
+    <sheet name="profile" sheetId="2" r:id="rId11"/>
+    <sheet name="homePage" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="639">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1885,6 +1886,84 @@
   </si>
   <si>
     <t>Amount must be more than or equal to $5.00 USD</t>
+  </si>
+  <si>
+    <t>bankHeading</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>last4Digits</t>
+  </si>
+  <si>
+    <t>avalible</t>
+  </si>
+  <si>
+    <t>sucessHeading</t>
+  </si>
+  <si>
+    <t>removeHeading</t>
+  </si>
+  <si>
+    <t>test withdrawn to External Bank</t>
+  </si>
+  <si>
+    <t>external bank</t>
+  </si>
+  <si>
+    <t>Withdraw to Bank Account</t>
+  </si>
+  <si>
+    <t>CashEdge Test</t>
+  </si>
+  <si>
+    <t>Available Balance:</t>
+  </si>
+  <si>
+    <t>Please allow 3-5 business days to process this transaction.</t>
+  </si>
+  <si>
+    <t>test withdrawn to External Bank Remove</t>
+  </si>
+  <si>
+    <t>Remove external bank</t>
+  </si>
+  <si>
+    <t>Remove Payment Method</t>
+  </si>
+  <si>
+    <t>Amount is required</t>
+  </si>
+  <si>
+    <t>Payment Method Removed Successfully</t>
+  </si>
+  <si>
+    <t>test withdrawn to External Bank invalid amount</t>
+  </si>
+  <si>
+    <t>min Amount</t>
+  </si>
+  <si>
+    <t>Insufficient funds</t>
+  </si>
+  <si>
+    <t>test withdrawn to External Bank Remove1</t>
+  </si>
+  <si>
+    <t>Remove external bank1</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>removeHeading1</t>
+  </si>
+  <si>
+    <t>4219</t>
+  </si>
+  <si>
+    <t>3456</t>
   </si>
 </sst>
 </file>
@@ -3126,6 +3205,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3140,7 +3236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B18C423-D7E7-4B7B-9167-D2BDC190AA4E}">
   <dimension ref="A1:W22"/>
   <sheetViews>
@@ -5420,7 +5516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0341D91D-2664-4CF3-AF4B-EBD6A1B18156}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -6254,6 +6350,365 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDACEBAE-0399-44B8-918C-9E44A81E28E5}">
+  <dimension ref="A1:U7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" customWidth="1"/>
+    <col min="19" max="19" width="15.109375" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B2" t="s">
+        <v>620</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F2" t="s">
+        <v>564</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>622</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="N2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O2" t="s">
+        <v>243</v>
+      </c>
+      <c r="P2" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>226</v>
+      </c>
+      <c r="R2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F3" t="s">
+        <v>564</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="S3" t="s">
+        <v>627</v>
+      </c>
+      <c r="T3" t="s">
+        <v>628</v>
+      </c>
+      <c r="U3" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>630</v>
+      </c>
+      <c r="B4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F4" t="s">
+        <v>564</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>621</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>630</v>
+      </c>
+      <c r="B5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" t="s">
+        <v>564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>621</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="T5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>630</v>
+      </c>
+      <c r="B6" t="s">
+        <v>631</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F6" t="s">
+        <v>564</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>621</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="T6" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>633</v>
+      </c>
+      <c r="B7" t="s">
+        <v>634</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F7" t="s">
+        <v>564</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="S7" t="s">
+        <v>627</v>
+      </c>
+      <c r="U7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{93BAE2C2-8D83-48C0-A5FA-DB09CC9BA294}"/>
+    <hyperlink ref="E3:E7" r:id="rId2" display="Admin@123" xr:uid="{D63F3337-2163-4170-8DDA-0C1E908BA8AC}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{28974E15-D2FB-41E9-B38F-9DA305AE0B47}"/>
+    <hyperlink ref="D3:D7" r:id="rId4" display="maniv789396@gmail.com" xr:uid="{BBBCF58A-9ACB-4AFB-932C-17CD8D29B2F1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D06DFA-D6F9-4A05-B463-4DDA52F0E3E7}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
@@ -7696,7 +8151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7342C061-16F1-49A5-BA07-4D17E62E882D}">
   <dimension ref="A1:AM42"/>
   <sheetViews>
@@ -9730,7 +10185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F2C328-44FE-4BE7-9D79-D8AE6FF7329F}">
   <dimension ref="A1:S15"/>
   <sheetViews>
@@ -10283,7 +10738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD7EB4D-1B81-49AC-A852-CF79C3CF942B}">
   <dimension ref="A1:X18"/>
   <sheetViews>
@@ -11506,21 +11961,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>